<commit_message>
Updated technical validation to work with .xlsx instead of .xls file type
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <bookViews>
-    <workbookView activeTab="79"/>
+    <workbookView activeTab="80"/>
   </bookViews>
   <sheets>
     <sheet state="visible" name="12000053001" sheetId="1" r:id="rId4"/>
@@ -13766,7 +13766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A1" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M27" sqref="M27"/>
+      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -13781,7 +13781,7 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="257" width="9.42578125" customWidth="1"/>
+    <col min="11" max="251" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -14209,9 +14209,6 @@
       </c>
       <c r="L12" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13">
@@ -16701,7 +16698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A1" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="topLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -16716,7 +16713,7 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="257" width="9.42578125" customWidth="1"/>
+    <col min="11" max="256" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -17144,9 +17141,6 @@
       </c>
       <c r="L12" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13">
@@ -17792,7 +17786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A1" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O30" sqref="O30"/>
+      <selection pane="topLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -17807,7 +17801,7 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="257" width="9.42578125" customWidth="1"/>
+    <col min="11" max="256" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -18235,9 +18229,6 @@
       </c>
       <c r="L12" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13">
@@ -30189,7 +30180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A1" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="topLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -30204,7 +30195,7 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="257" width="9.42578125" customWidth="1"/>
+    <col min="11" max="252" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -30732,8 +30723,6 @@
       <c r="L15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="3"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
@@ -30772,7 +30761,6 @@
       <c r="L16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
@@ -30811,15 +30799,12 @@
       <c r="L17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="3"/>
     </row>
     <row r="19">
       <c r="A19" s="1"/>
@@ -30833,8 +30818,6 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="5"/>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
@@ -30848,7 +30831,6 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
-      <c r="N20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="1"/>
@@ -30863,7 +30845,6 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="N21" s="2"/>
     </row>
   </sheetData>
 </worksheet>
@@ -30873,7 +30854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A1" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L21" sqref="L21"/>
+      <selection pane="topLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -30888,7 +30869,7 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="257" width="9.42578125" customWidth="1"/>
+    <col min="11" max="253" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -34379,7 +34360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A1" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M30" sqref="M30"/>
+      <selection pane="topLeft" activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -37092,7 +37073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A1" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I30" sqref="I30"/>
+      <selection pane="topLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -37107,7 +37088,7 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="257" width="9.42578125" customWidth="1"/>
+    <col min="11" max="256" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -37182,26 +37163,26 @@
       <c r="D3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1">
-        <v>18</v>
+      <c r="E3" s="0">
+        <v>6</v>
+      </c>
+      <c r="F3" s="0">
+        <v>9</v>
+      </c>
+      <c r="G3" s="0">
+        <v>16</v>
+      </c>
+      <c r="H3" s="0">
+        <v>21</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
       </c>
-      <c r="J3" s="1">
-        <v>4</v>
-      </c>
-      <c r="K3" s="1">
-        <v>13.8</v>
+      <c r="J3" s="0">
+        <v>6</v>
+      </c>
+      <c r="K3" s="0">
+        <v>26.8</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>19</v>
@@ -37220,26 +37201,26 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="1">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="H4" s="1">
-        <v>12</v>
+      <c r="E4" s="0">
+        <v>6</v>
+      </c>
+      <c r="F4" s="0">
+        <v>9</v>
+      </c>
+      <c r="G4" s="0">
+        <v>14</v>
+      </c>
+      <c r="H4" s="0">
+        <v>16</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
       </c>
-      <c r="J4" s="1">
-        <v>4</v>
-      </c>
-      <c r="K4" s="1">
-        <v>11.39</v>
+      <c r="J4" s="0">
+        <v>6</v>
+      </c>
+      <c r="K4" s="0">
+        <v>5.32</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>19</v>
@@ -37258,26 +37239,26 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1">
-        <v>18</v>
-      </c>
-      <c r="H5" s="1">
-        <v>21.5</v>
+      <c r="E5" s="0">
+        <v>6</v>
+      </c>
+      <c r="F5" s="0">
+        <v>9</v>
+      </c>
+      <c r="G5" s="0">
+        <v>21</v>
+      </c>
+      <c r="H5" s="0">
+        <v>23</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="J5" s="1">
-        <v>4</v>
-      </c>
-      <c r="K5" s="1">
-        <v>11.39</v>
+      <c r="J5" s="0">
+        <v>6</v>
+      </c>
+      <c r="K5" s="0">
+        <v>5.32</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>19</v>
@@ -37296,10 +37277,10 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="E6" s="0">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0">
         <v>12</v>
       </c>
       <c r="G6" s="1">
@@ -37314,8 +37295,8 @@
       <c r="J6" s="1">
         <v>6</v>
       </c>
-      <c r="K6" s="1">
-        <v>22.55</v>
+      <c r="K6" s="0">
+        <v>20.7</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>19</v>
@@ -37328,32 +37309,32 @@
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>38</v>
+      <c r="C7" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>4</v>
-      </c>
-      <c r="G7" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="H7" s="1">
-        <v>21.5</v>
+      <c r="E7" s="0">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0">
+        <v>5</v>
+      </c>
+      <c r="G7" s="0">
+        <v>16</v>
+      </c>
+      <c r="H7" s="0">
+        <v>21</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
       </c>
-      <c r="J7" s="1">
-        <v>4</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0</v>
+      <c r="J7" s="0">
+        <v>6</v>
+      </c>
+      <c r="K7" s="0">
+        <v>1.78</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>19</v>
@@ -37366,32 +37347,32 @@
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>39</v>
+      <c r="C8" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
       </c>
-      <c r="E8" s="1">
-        <v>11</v>
+      <c r="E8" s="0">
+        <v>10</v>
       </c>
       <c r="F8" s="1">
         <v>12</v>
       </c>
-      <c r="G8" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="H8" s="1">
-        <v>21.5</v>
+      <c r="G8" s="0">
+        <v>16</v>
+      </c>
+      <c r="H8" s="0">
+        <v>21</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
       </c>
-      <c r="J8" s="1">
-        <v>4</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0</v>
+      <c r="J8" s="0">
+        <v>6</v>
+      </c>
+      <c r="K8" s="0">
+        <v>1.78</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>19</v>
@@ -37407,26 +37388,26 @@
       <c r="D9" s="1">
         <v>0</v>
       </c>
-      <c r="E9" s="1">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1">
-        <v>10</v>
+      <c r="E9" s="0">
+        <v>6</v>
+      </c>
+      <c r="F9" s="0">
+        <v>9</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="1">
-        <v>8.5</v>
+      <c r="H9" s="0">
+        <v>14</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="1">
-        <v>4</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0.09885</v>
+      <c r="J9" s="0">
+        <v>6</v>
+      </c>
+      <c r="K9" s="0">
+        <v>0.09816</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>16</v>
@@ -37442,26 +37423,26 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" s="1">
-        <v>5</v>
-      </c>
-      <c r="F10" s="1">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="H10" s="1">
-        <v>21.5</v>
+      <c r="E10" s="0">
+        <v>6</v>
+      </c>
+      <c r="F10" s="0">
+        <v>9</v>
+      </c>
+      <c r="G10" s="0">
+        <v>14</v>
+      </c>
+      <c r="H10" s="0">
+        <v>16</v>
       </c>
       <c r="I10" s="1">
         <v>0</v>
       </c>
-      <c r="J10" s="1">
-        <v>4</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0.10462</v>
+      <c r="J10" s="0">
+        <v>6</v>
+      </c>
+      <c r="K10" s="0">
+        <v>0.11735</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>16</v>
@@ -37477,26 +37458,26 @@
       <c r="D11" s="1">
         <v>0</v>
       </c>
-      <c r="E11" s="1">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1">
-        <v>10</v>
-      </c>
-      <c r="G11" s="1">
-        <v>21.5</v>
-      </c>
-      <c r="H11" s="1">
-        <v>24</v>
+      <c r="E11" s="0">
+        <v>6</v>
+      </c>
+      <c r="F11" s="0">
+        <v>9</v>
+      </c>
+      <c r="G11" s="0">
+        <v>16</v>
+      </c>
+      <c r="H11" s="0">
+        <v>21</v>
       </c>
       <c r="I11" s="1">
         <v>0</v>
       </c>
-      <c r="J11" s="1">
-        <v>4</v>
-      </c>
-      <c r="K11" s="1">
-        <v>0.09885</v>
+      <c r="J11" s="0">
+        <v>6</v>
+      </c>
+      <c r="K11" s="0">
+        <v>0.14484</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>16</v>
@@ -37512,32 +37493,29 @@
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="1">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1">
-        <v>10</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>24</v>
+      <c r="E12" s="0">
+        <v>6</v>
+      </c>
+      <c r="F12" s="0">
+        <v>9</v>
+      </c>
+      <c r="G12" s="0">
+        <v>21</v>
+      </c>
+      <c r="H12" s="0">
+        <v>23</v>
       </c>
       <c r="I12" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1">
         <v>6</v>
       </c>
-      <c r="K12" s="1">
-        <v>0.09885</v>
+      <c r="K12" s="0">
+        <v>0.11735</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13">
@@ -37550,26 +37528,26 @@
       <c r="D13" s="1">
         <v>0</v>
       </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
-        <v>4</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>8.5</v>
+      <c r="E13" s="0">
+        <v>6</v>
+      </c>
+      <c r="F13" s="0">
+        <v>9</v>
+      </c>
+      <c r="G13" s="0">
+        <v>23</v>
+      </c>
+      <c r="H13" s="0">
+        <v>24</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
       </c>
       <c r="J13" s="1">
-        <v>4</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0.08468</v>
+        <v>6</v>
+      </c>
+      <c r="K13" s="0">
+        <v>0.09816</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>16</v>
@@ -37588,23 +37566,23 @@
       <c r="E14" s="1">
         <v>1</v>
       </c>
-      <c r="F14" s="1">
-        <v>4</v>
+      <c r="F14" s="0">
+        <v>2</v>
       </c>
       <c r="G14" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="H14" s="1">
-        <v>21.5</v>
+        <v>0</v>
+      </c>
+      <c r="H14" s="0">
+        <v>16</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
       </c>
-      <c r="J14" s="1">
-        <v>4</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0.08534</v>
+      <c r="J14" s="0">
+        <v>6</v>
+      </c>
+      <c r="K14" s="0">
+        <v>0.09822</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>16</v>
@@ -37623,23 +37601,23 @@
       <c r="E15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="1">
-        <v>4</v>
-      </c>
-      <c r="G15" s="1">
-        <v>21.5</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="F15" s="0">
+        <v>2</v>
+      </c>
+      <c r="G15" s="0">
+        <v>21</v>
+      </c>
+      <c r="H15" s="0">
         <v>24</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
       </c>
-      <c r="J15" s="1">
-        <v>4</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0.08468</v>
+      <c r="J15" s="0">
+        <v>6</v>
+      </c>
+      <c r="K15" s="0">
+        <v>0.09822</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>16</v>
@@ -37655,26 +37633,26 @@
       <c r="D16" s="1">
         <v>0</v>
       </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1">
-        <v>4</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>24</v>
+      <c r="E16" s="0">
+        <v>1</v>
+      </c>
+      <c r="F16" s="0">
+        <v>5</v>
+      </c>
+      <c r="G16" s="0">
+        <v>16</v>
+      </c>
+      <c r="H16" s="0">
+        <v>21</v>
       </c>
       <c r="I16" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J16" s="1">
         <v>6</v>
       </c>
-      <c r="K16" s="1">
-        <v>0.08468</v>
+      <c r="K16" s="0">
+        <v>0.12734</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>16</v>
@@ -37690,26 +37668,26 @@
       <c r="D17" s="1">
         <v>0</v>
       </c>
-      <c r="E17" s="1">
-        <v>11</v>
-      </c>
-      <c r="F17" s="1">
-        <v>12</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>8.5</v>
+      <c r="E17" s="0">
+        <v>3</v>
+      </c>
+      <c r="F17" s="0">
+        <v>5</v>
+      </c>
+      <c r="G17" s="0">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0">
+        <v>9</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
       </c>
       <c r="J17" s="1">
-        <v>4</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0.08468</v>
+        <v>6</v>
+      </c>
+      <c r="K17" s="0">
+        <v>0.09822</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>16</v>
@@ -37725,26 +37703,26 @@
       <c r="D18" s="1">
         <v>0</v>
       </c>
-      <c r="E18" s="1">
-        <v>11</v>
-      </c>
-      <c r="F18" s="1">
-        <v>12</v>
-      </c>
-      <c r="G18" s="1">
-        <v>8.5</v>
-      </c>
-      <c r="H18" s="1">
-        <v>21.5</v>
+      <c r="E18" s="0">
+        <v>3</v>
+      </c>
+      <c r="F18" s="0">
+        <v>5</v>
+      </c>
+      <c r="G18" s="0">
+        <v>9</v>
+      </c>
+      <c r="H18" s="0">
+        <v>14</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
       </c>
       <c r="J18" s="1">
-        <v>4</v>
-      </c>
-      <c r="K18" s="1">
-        <v>0.08534</v>
+        <v>6</v>
+      </c>
+      <c r="K18" s="0">
+        <v>0.0569</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>16</v>
@@ -37760,26 +37738,26 @@
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="1">
-        <v>11</v>
-      </c>
-      <c r="F19" s="1">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1">
-        <v>21.5</v>
-      </c>
-      <c r="H19" s="1">
-        <v>24</v>
+      <c r="E19" s="0">
+        <v>3</v>
+      </c>
+      <c r="F19" s="0">
+        <v>5</v>
+      </c>
+      <c r="G19" s="0">
+        <v>14</v>
+      </c>
+      <c r="H19" s="0">
+        <v>16</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
       </c>
-      <c r="J19" s="1">
-        <v>4</v>
-      </c>
-      <c r="K19" s="1">
-        <v>0.08468</v>
+      <c r="J19" s="0">
+        <v>6</v>
+      </c>
+      <c r="K19" s="0">
+        <v>0.09822</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>16</v>
@@ -37795,26 +37773,26 @@
       <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="E20" s="1">
-        <v>11</v>
-      </c>
-      <c r="F20" s="1">
-        <v>12</v>
-      </c>
-      <c r="G20" s="1">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1">
+      <c r="E20" s="0">
+        <v>3</v>
+      </c>
+      <c r="F20" s="0">
+        <v>5</v>
+      </c>
+      <c r="G20" s="0">
+        <v>21</v>
+      </c>
+      <c r="H20" s="0">
         <v>24</v>
       </c>
       <c r="I20" s="1">
-        <v>5</v>
-      </c>
-      <c r="J20" s="1">
-        <v>6</v>
-      </c>
-      <c r="K20" s="1">
-        <v>0.08468</v>
+        <v>0</v>
+      </c>
+      <c r="J20" s="0">
+        <v>6</v>
+      </c>
+      <c r="K20" s="0">
+        <v>0.09822</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>16</v>
@@ -37822,92 +37800,110 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K21" s="1">
-        <f>30*4.95518</f>
-        <v>148.6554</v>
+        <v>15</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0">
+        <v>16</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>6</v>
+      </c>
+      <c r="K21" s="0">
+        <v>0.09822</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>40</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="M21" s="0"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3">
-        <v>1</v>
-      </c>
-      <c r="F22" s="3">
-        <v>3</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3">
-        <v>24</v>
-      </c>
-      <c r="I22" s="3">
-        <v>0</v>
-      </c>
-      <c r="J22" s="3">
-        <v>6</v>
-      </c>
-      <c r="K22" s="3">
-        <v>1.68736</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>24</v>
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="0"/>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1">
+        <v>12</v>
+      </c>
+      <c r="G22" s="0">
+        <v>21</v>
+      </c>
+      <c r="H22" s="0">
+        <v>24</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>6</v>
+      </c>
+      <c r="K22" s="0">
+        <v>0.09822</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3">
-        <v>4</v>
-      </c>
-      <c r="F23" s="3">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="0"/>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0">
         <v>10</v>
       </c>
-      <c r="G23" s="3">
-        <v>0</v>
-      </c>
-      <c r="H23" s="3">
-        <v>24</v>
-      </c>
-      <c r="I23" s="3">
-        <v>0</v>
-      </c>
-      <c r="J23" s="3">
-        <v>6</v>
-      </c>
-      <c r="K23" s="3">
-        <v>1.54031</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>24</v>
+      <c r="F23" s="1">
+        <v>12</v>
+      </c>
+      <c r="G23" s="0">
+        <v>16</v>
+      </c>
+      <c r="H23" s="0">
+        <v>21</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>6</v>
+      </c>
+      <c r="K23" s="0">
+        <v>0.12734</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="24">
@@ -37915,35 +37911,24 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="3">
-        <v>0</v>
-      </c>
-      <c r="E24" s="3">
-        <v>11</v>
-      </c>
-      <c r="F24" s="3">
-        <v>12</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0</v>
-      </c>
-      <c r="H24" s="3">
-        <v>24</v>
-      </c>
-      <c r="I24" s="3">
-        <v>0</v>
-      </c>
-      <c r="J24" s="3">
-        <v>6</v>
-      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
       <c r="K24" s="3">
-        <v>1.68736</v>
+        <v>148.6554</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25">
@@ -37955,7 +37940,7 @@
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
@@ -37976,11 +37961,12 @@
         <v>6</v>
       </c>
       <c r="K25" s="3">
-        <v>1.3126</v>
+        <v>1.68736</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="M25" s="3"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
@@ -37991,7 +37977,7 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="E26" s="3">
         <v>4</v>
@@ -38012,11 +37998,12 @@
         <v>6</v>
       </c>
       <c r="K26" s="3">
-        <v>1.22418</v>
+        <v>1.54031</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="M26" s="3"/>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
@@ -38027,7 +38014,7 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3">
-        <v>4000</v>
+        <v>0</v>
       </c>
       <c r="E27" s="3">
         <v>11</v>
@@ -38048,11 +38035,123 @@
         <v>6</v>
       </c>
       <c r="K27" s="3">
+        <v>1.68736</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3">
+        <v>4000</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3">
+        <v>3</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>24</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>6</v>
+      </c>
+      <c r="K28" s="3">
         <v>1.3126</v>
       </c>
-      <c r="L27" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="L28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3">
+        <v>4000</v>
+      </c>
+      <c r="E29" s="3">
+        <v>4</v>
+      </c>
+      <c r="F29" s="3">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>24</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>6</v>
+      </c>
+      <c r="K29" s="3">
+        <v>1.22418</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="3"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3">
+        <v>4000</v>
+      </c>
+      <c r="E30" s="3">
+        <v>11</v>
+      </c>
+      <c r="F30" s="3">
+        <v>12</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>24</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>6</v>
+      </c>
+      <c r="K30" s="3">
+        <v>1.3126</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" s="3"/>
     </row>
   </sheetData>
 </worksheet>
@@ -41518,167 +41617,186 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="0">
-        <v>204.05</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="K2" s="1">
+        <f>50.48874*30</f>
+        <v>1514.6622</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="M2" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="0">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1">
         <v>0</v>
       </c>
       <c r="E3" s="0">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F3" s="0">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G3" s="0">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H3" s="0">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0">
+        <v>6</v>
+      </c>
+      <c r="K3" s="0">
+        <v>26.8</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="0">
+        <v>6</v>
+      </c>
+      <c r="F4" s="0">
         <v>9</v>
       </c>
-      <c r="I3" s="0">
-        <v>0</v>
-      </c>
-      <c r="J3" s="0">
-        <v>6</v>
-      </c>
-      <c r="K3" s="0">
-        <v>0.0965</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="0">
-        <v>0</v>
-      </c>
-      <c r="E4" s="0">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0">
-        <v>5</v>
-      </c>
       <c r="G4" s="0">
+        <v>14</v>
+      </c>
+      <c r="H4" s="0">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="0">
+        <v>6</v>
+      </c>
+      <c r="K4" s="0">
+        <v>5.32</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="0">
+        <v>6</v>
+      </c>
+      <c r="F5" s="0">
         <v>9</v>
       </c>
-      <c r="H4" s="0">
-        <v>16</v>
-      </c>
-      <c r="I4" s="0">
-        <v>0</v>
-      </c>
-      <c r="J4" s="0">
-        <v>6</v>
-      </c>
-      <c r="K4" s="0">
-        <v>0.0832</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="0">
-        <v>0</v>
-      </c>
-      <c r="E5" s="0">
-        <v>1</v>
-      </c>
-      <c r="F5" s="0">
-        <v>5</v>
-      </c>
       <c r="G5" s="0">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H5" s="0">
-        <v>21</v>
-      </c>
-      <c r="I5" s="0">
+        <v>23</v>
+      </c>
+      <c r="I5" s="1">
         <v>0</v>
       </c>
       <c r="J5" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K5" s="0">
-        <v>0.1205</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>16</v>
+        <v>5.32</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="0">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1">
         <v>0</v>
       </c>
       <c r="E6" s="0">
         <v>1</v>
       </c>
       <c r="F6" s="0">
-        <v>5</v>
-      </c>
-      <c r="G6" s="0">
-        <v>21</v>
-      </c>
-      <c r="H6" s="0">
-        <v>24</v>
-      </c>
-      <c r="I6" s="0">
-        <v>0</v>
-      </c>
-      <c r="J6" s="0">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>24</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
         <v>6</v>
       </c>
       <c r="K6" s="0">
-        <v>0.0965</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>16</v>
+        <v>20.7</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="0">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1">
         <v>0</v>
       </c>
       <c r="E7" s="0">
@@ -41693,62 +41811,65 @@
       <c r="H7" s="0">
         <v>21</v>
       </c>
-      <c r="I7" s="0">
-        <v>5</v>
+      <c r="I7" s="1">
+        <v>0</v>
       </c>
       <c r="J7" s="0">
         <v>6</v>
       </c>
       <c r="K7" s="0">
-        <v>0.0965</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>16</v>
+        <v>1.78</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="0">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1">
         <v>0</v>
       </c>
       <c r="E8" s="0">
-        <v>6</v>
-      </c>
-      <c r="F8" s="0">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F8" s="1">
+        <v>12</v>
       </c>
       <c r="G8" s="0">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H8" s="0">
-        <v>16</v>
-      </c>
-      <c r="I8" s="0">
+        <v>21</v>
+      </c>
+      <c r="I8" s="1">
         <v>0</v>
       </c>
       <c r="J8" s="0">
         <v>6</v>
       </c>
       <c r="K8" s="0">
-        <v>0.1078</v>
-      </c>
-      <c r="L8" s="0" t="s">
-        <v>16</v>
+        <v>1.78</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="0">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1">
         <v>0</v>
       </c>
       <c r="E9" s="0">
@@ -41757,33 +41878,33 @@
       <c r="F9" s="0">
         <v>9</v>
       </c>
-      <c r="G9" s="0">
-        <v>16</v>
+      <c r="G9" s="1">
+        <v>0</v>
       </c>
       <c r="H9" s="0">
-        <v>21</v>
-      </c>
-      <c r="I9" s="0">
+        <v>14</v>
+      </c>
+      <c r="I9" s="1">
         <v>0</v>
       </c>
       <c r="J9" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K9" s="0">
-        <v>0.1733</v>
-      </c>
-      <c r="L9" s="0" t="s">
+        <v>0.09816</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="0">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1">
         <v>0</v>
       </c>
       <c r="E10" s="0">
@@ -41793,32 +41914,32 @@
         <v>9</v>
       </c>
       <c r="G10" s="0">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H10" s="0">
-        <v>24</v>
-      </c>
-      <c r="I10" s="0">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1">
         <v>0</v>
       </c>
       <c r="J10" s="0">
         <v>6</v>
       </c>
       <c r="K10" s="0">
-        <v>0.1078</v>
-      </c>
-      <c r="L10" s="0" t="s">
+        <v>0.11735</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="0">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1">
         <v>0</v>
       </c>
       <c r="E11" s="0">
@@ -41833,139 +41954,139 @@
       <c r="H11" s="0">
         <v>21</v>
       </c>
-      <c r="I11" s="0">
-        <v>5</v>
+      <c r="I11" s="1">
+        <v>0</v>
       </c>
       <c r="J11" s="0">
         <v>6</v>
       </c>
       <c r="K11" s="0">
-        <v>0.1078</v>
-      </c>
-      <c r="L11" s="0" t="s">
+        <v>0.14484</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="0">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1">
         <v>0</v>
       </c>
       <c r="E12" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F12" s="0">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G12" s="0">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="H12" s="0">
+        <v>23</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>6</v>
+      </c>
+      <c r="K12" s="0">
+        <v>0.11735</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="0">
+        <v>6</v>
+      </c>
+      <c r="F13" s="0">
         <v>9</v>
       </c>
-      <c r="I12" s="0">
-        <v>0</v>
-      </c>
-      <c r="J12" s="0">
-        <v>6</v>
-      </c>
-      <c r="K12" s="0">
-        <v>0.0965</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="0">
-        <v>0</v>
-      </c>
-      <c r="E13" s="0">
-        <v>10</v>
-      </c>
-      <c r="F13" s="0">
-        <v>12</v>
-      </c>
       <c r="G13" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="H13" s="0">
-        <v>16</v>
-      </c>
-      <c r="I13" s="0">
-        <v>0</v>
-      </c>
-      <c r="J13" s="0">
+        <v>24</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
         <v>6</v>
       </c>
       <c r="K13" s="0">
-        <v>0.0832</v>
-      </c>
-      <c r="L13" s="0" t="s">
+        <v>0.09816</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="0">
-        <v>0</v>
-      </c>
-      <c r="E14" s="0">
-        <v>10</v>
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
       </c>
       <c r="F14" s="0">
-        <v>12</v>
-      </c>
-      <c r="G14" s="0">
-        <v>16</v>
+        <v>2</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
       </c>
       <c r="H14" s="0">
-        <v>21</v>
-      </c>
-      <c r="I14" s="0">
+        <v>16</v>
+      </c>
+      <c r="I14" s="1">
         <v>0</v>
       </c>
       <c r="J14" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K14" s="0">
-        <v>0.1205</v>
-      </c>
-      <c r="L14" s="0" t="s">
+        <v>0.09822</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="0">
-        <v>0</v>
-      </c>
-      <c r="E15" s="0">
-        <v>10</v>
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
       </c>
       <c r="F15" s="0">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G15" s="0">
         <v>21</v>
@@ -41973,34 +42094,34 @@
       <c r="H15" s="0">
         <v>24</v>
       </c>
-      <c r="I15" s="0">
+      <c r="I15" s="1">
         <v>0</v>
       </c>
       <c r="J15" s="0">
         <v>6</v>
       </c>
       <c r="K15" s="0">
-        <v>0.0965</v>
-      </c>
-      <c r="L15" s="0" t="s">
+        <v>0.09822</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="0">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1">
         <v>0</v>
       </c>
       <c r="E16" s="0">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F16" s="0">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G16" s="0">
         <v>16</v>
@@ -42008,304 +42129,516 @@
       <c r="H16" s="0">
         <v>21</v>
       </c>
-      <c r="I16" s="0">
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>6</v>
+      </c>
+      <c r="K16" s="0">
+        <v>0.12734</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="0"/>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0">
+        <v>3</v>
+      </c>
+      <c r="F17" s="0">
         <v>5</v>
       </c>
-      <c r="J16" s="0">
-        <v>6</v>
-      </c>
-      <c r="K16" s="0">
-        <v>0.0965</v>
-      </c>
-      <c r="L16" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="0">
-        <v>0</v>
-      </c>
-      <c r="E17" s="0">
-        <v>6</v>
-      </c>
-      <c r="F17" s="0">
+      <c r="G17" s="0">
+        <v>0</v>
+      </c>
+      <c r="H17" s="0">
         <v>9</v>
       </c>
-      <c r="G17" s="0">
-        <v>16</v>
-      </c>
-      <c r="H17" s="0">
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>6</v>
+      </c>
+      <c r="K17" s="0">
+        <v>0.09822</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="0"/>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0">
+        <v>3</v>
+      </c>
+      <c r="F18" s="0">
+        <v>5</v>
+      </c>
+      <c r="G18" s="0">
+        <v>9</v>
+      </c>
+      <c r="H18" s="0">
+        <v>14</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>6</v>
+      </c>
+      <c r="K18" s="0">
+        <v>0.0569</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0">
+        <v>3</v>
+      </c>
+      <c r="F19" s="0">
+        <v>5</v>
+      </c>
+      <c r="G19" s="0">
+        <v>14</v>
+      </c>
+      <c r="H19" s="0">
+        <v>16</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="0">
+        <v>6</v>
+      </c>
+      <c r="K19" s="0">
+        <v>0.09822</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M19" s="0"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0">
+        <v>3</v>
+      </c>
+      <c r="F20" s="0">
+        <v>5</v>
+      </c>
+      <c r="G20" s="0">
         <v>21</v>
       </c>
-      <c r="I17" s="0">
-        <v>0</v>
-      </c>
-      <c r="J17" s="0">
-        <v>4</v>
-      </c>
-      <c r="K17" s="0">
-        <v>4.93</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="0">
-        <v>0</v>
-      </c>
-      <c r="E18" s="0">
-        <v>1</v>
-      </c>
-      <c r="F18" s="0">
-        <v>12</v>
-      </c>
-      <c r="G18" s="0">
-        <v>0</v>
-      </c>
-      <c r="H18" s="0">
-        <v>24</v>
-      </c>
-      <c r="I18" s="0">
-        <v>0</v>
-      </c>
-      <c r="J18" s="0">
-        <v>6</v>
-      </c>
-      <c r="K18" s="0">
-        <v>4.3</v>
-      </c>
-      <c r="L18" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0" t="s">
+      <c r="H20" s="0">
+        <v>24</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="0">
+        <v>6</v>
+      </c>
+      <c r="K20" s="0">
+        <v>0.09822</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0">
+        <v>16</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>6</v>
+      </c>
+      <c r="K21" s="0">
+        <v>0.09822</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M21" s="0"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="0"/>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1">
+        <v>12</v>
+      </c>
+      <c r="G22" s="0">
+        <v>21</v>
+      </c>
+      <c r="H22" s="0">
+        <v>24</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>6</v>
+      </c>
+      <c r="K22" s="0">
+        <v>0.09822</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="0"/>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="0">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1">
+        <v>12</v>
+      </c>
+      <c r="G23" s="0">
+        <v>16</v>
+      </c>
+      <c r="H23" s="0">
+        <v>21</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>6</v>
+      </c>
+      <c r="K23" s="0">
+        <v>0.12734</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K19" s="0">
-        <f>30*4.95518</f>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3">
         <v>148.6554</v>
       </c>
-      <c r="L19" s="0" t="s">
+      <c r="L24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M19" s="0" t="s">
+      <c r="M24" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="0" t="s">
+    <row r="25">
+      <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="0">
-        <v>0</v>
-      </c>
-      <c r="E20" s="0">
-        <v>1</v>
-      </c>
-      <c r="F20" s="0">
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
         <v>3</v>
       </c>
-      <c r="G20" s="0">
-        <v>0</v>
-      </c>
-      <c r="H20" s="0">
-        <v>24</v>
-      </c>
-      <c r="I20" s="0">
-        <v>0</v>
-      </c>
-      <c r="J20" s="0">
-        <v>6</v>
-      </c>
-      <c r="L20" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="0" t="s">
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>24</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>6</v>
+      </c>
+      <c r="K25" s="3">
+        <v>1.68736</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="0">
+      <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3">
+        <v>10</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>24</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
+      <c r="J26" s="3">
+        <v>6</v>
+      </c>
+      <c r="K26" s="3">
+        <v>1.54031</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" s="3"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>11</v>
+      </c>
+      <c r="F27" s="3">
+        <v>12</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>24</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
+      <c r="J27" s="3">
+        <v>6</v>
+      </c>
+      <c r="K27" s="3">
+        <v>1.68736</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3">
         <v>4000</v>
       </c>
-      <c r="E21" s="0">
-        <v>1</v>
-      </c>
-      <c r="F21" s="0">
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3">
         <v>3</v>
       </c>
-      <c r="G21" s="0">
-        <v>0</v>
-      </c>
-      <c r="H21" s="0">
-        <v>24</v>
-      </c>
-      <c r="I21" s="0">
-        <v>0</v>
-      </c>
-      <c r="J21" s="0">
-        <v>6</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="0" t="s">
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>24</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>6</v>
+      </c>
+      <c r="K28" s="3">
+        <v>1.3126</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="0">
-        <v>0</v>
-      </c>
-      <c r="E22" s="0">
-        <v>4</v>
-      </c>
-      <c r="F22" s="0">
+      <c r="B29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3">
+        <v>4000</v>
+      </c>
+      <c r="E29" s="3">
+        <v>4</v>
+      </c>
+      <c r="F29" s="3">
         <v>10</v>
       </c>
-      <c r="G22" s="0">
-        <v>0</v>
-      </c>
-      <c r="H22" s="0">
-        <v>24</v>
-      </c>
-      <c r="I22" s="0">
-        <v>0</v>
-      </c>
-      <c r="J22" s="0">
-        <v>6</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="0" t="s">
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>24</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>6</v>
+      </c>
+      <c r="K29" s="3">
+        <v>1.22418</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="3"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="0">
+      <c r="B30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3">
         <v>4000</v>
       </c>
-      <c r="E23" s="0">
-        <v>4</v>
-      </c>
-      <c r="F23" s="0">
-        <v>10</v>
-      </c>
-      <c r="G23" s="0">
-        <v>0</v>
-      </c>
-      <c r="H23" s="0">
-        <v>24</v>
-      </c>
-      <c r="I23" s="0">
-        <v>0</v>
-      </c>
-      <c r="J23" s="0">
-        <v>6</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="0">
-        <v>0</v>
-      </c>
-      <c r="E24" s="0">
+      <c r="E30" s="3">
         <v>11</v>
       </c>
-      <c r="F24" s="0">
-        <v>12</v>
-      </c>
-      <c r="G24" s="0">
-        <v>0</v>
-      </c>
-      <c r="H24" s="0">
-        <v>24</v>
-      </c>
-      <c r="I24" s="0">
-        <v>0</v>
-      </c>
-      <c r="J24" s="0">
-        <v>6</v>
-      </c>
-      <c r="L24" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="0">
-        <v>4000</v>
-      </c>
-      <c r="E25" s="0">
-        <v>11</v>
-      </c>
-      <c r="F25" s="0">
-        <v>12</v>
-      </c>
-      <c r="G25" s="0">
-        <v>0</v>
-      </c>
-      <c r="H25" s="0">
-        <v>24</v>
-      </c>
-      <c r="I25" s="0">
-        <v>0</v>
-      </c>
-      <c r="J25" s="0">
-        <v>6</v>
-      </c>
-      <c r="L25" s="0" t="s">
-        <v>24</v>
-      </c>
+      <c r="F30" s="3">
+        <v>12</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>24</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>6</v>
+      </c>
+      <c r="K30" s="3">
+        <v>1.3126</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" s="3"/>
     </row>
   </sheetData>
 </worksheet>
@@ -42315,7 +42648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A1" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I26" sqref="I26"/>
+      <selection pane="topLeft" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -42330,7 +42663,7 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="257" width="9.42578125" customWidth="1"/>
+    <col min="11" max="255" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -42766,9 +43099,6 @@
       </c>
       <c r="L12" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13">
@@ -48699,7 +49029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A1" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" sqref="C38"/>
+      <selection pane="topLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Got technical validation to work on metricated data
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-rates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169210BC-FC99-B044-B93A-1B7FF98DDA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CCE039-4FB6-6F44-9101-21D76B714782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="760" windowWidth="30240" windowHeight="17440" firstSheet="87" activeTab="90" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" firstSheet="53" activeTab="64" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5691" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5691" uniqueCount="91">
   <si>
     <t>utility</t>
   </si>
@@ -396,9 +396,6 @@
   </si>
   <si>
     <t>$/therm or $/m3</t>
-  </si>
-  <si>
-    <t>$/therm/hr  or $/m3/hr</t>
   </si>
   <si>
     <t>$/therm/hr or $/m3/hr</t>
@@ -827,7 +824,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -859,10 +856,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1879,10 +1876,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2188,10 +2185,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2478,10 +2475,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2769,10 +2766,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -3093,10 +3090,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -3624,10 +3621,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -4745,10 +4742,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -5130,10 +5127,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -5375,10 +5372,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -5906,10 +5903,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -6610,10 +6607,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -7141,10 +7138,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -7340,10 +7337,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -7843,10 +7840,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -8778,10 +8775,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -9693,10 +9690,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -9845,10 +9842,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -10172,10 +10169,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -10855,10 +10852,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -11101,10 +11098,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -11488,10 +11485,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -12524,10 +12521,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -13772,10 +13769,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -14157,10 +14154,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -15278,10 +15275,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -16312,7 +16309,7 @@
         <v>1.5403100000000001</v>
       </c>
       <c r="M26" s="7">
-        <f t="shared" ref="M26:M30" si="0">L26/2.83168</f>
+        <f t="shared" ref="M26:M29" si="0">L26/2.83168</f>
         <v>0.54395623799299364</v>
       </c>
       <c r="N26" t="s">
@@ -16533,10 +16530,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -16824,10 +16821,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -17194,10 +17191,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -17529,10 +17526,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -17833,7 +17830,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17865,10 +17862,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -18321,8 +18318,9 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="E12">
-        <v>3</v>
+      <c r="E12" s="10">
+        <f>D12*2.83168</f>
+        <v>8.4950399999999995</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -18481,10 +18479,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -18664,10 +18662,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -19918,10 +19916,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -21172,10 +21170,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -21835,10 +21833,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -22158,10 +22156,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -22904,10 +22902,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -23258,10 +23256,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -23549,10 +23547,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -23883,10 +23881,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -24069,10 +24067,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -24600,10 +24598,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -25090,10 +25088,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -25565,10 +25563,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -26237,7 +26235,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26269,10 +26267,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -26884,6 +26882,9 @@
       </c>
       <c r="C16" t="s">
         <v>28</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -26958,10 +26959,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -27609,7 +27610,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27641,10 +27642,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -28566,6 +28567,24 @@
       </c>
       <c r="E24">
         <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>24</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>6</v>
       </c>
       <c r="L24">
         <v>0.8</v>
@@ -28791,10 +28810,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -29768,10 +29787,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -30158,10 +30177,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -30690,10 +30709,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -30885,10 +30904,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -31918,7 +31937,7 @@
         <v>0.20305966775906881</v>
       </c>
       <c r="N25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -31963,10 +31982,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -32146,10 +32165,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -32341,10 +32360,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -32872,10 +32891,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -33188,10 +33207,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -33725,10 +33744,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -34221,10 +34240,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -34966,10 +34985,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -35711,10 +35730,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -35868,8 +35887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35900,10 +35919,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -36356,8 +36375,9 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="E12">
-        <v>3</v>
+      <c r="E12" s="10">
+        <f>D12*2.83168</f>
+        <v>8.4950399999999995</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -36516,10 +36536,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -36713,10 +36733,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -37746,7 +37766,7 @@
         <v>0.20305966775906881</v>
       </c>
       <c r="N25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -37790,10 +37810,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -38321,10 +38341,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -39032,10 +39052,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -40286,10 +40306,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -40621,10 +40641,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -42156,7 +42176,7 @@
         <v>3.0619632161826196E-2</v>
       </c>
       <c r="N38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -42201,10 +42221,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -43455,10 +43475,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -43641,10 +43661,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -43832,10 +43852,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -44306,10 +44326,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -44493,10 +44513,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -44864,7 +44884,7 @@
         <v>0.38846197310430558</v>
       </c>
       <c r="N10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -44909,10 +44929,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -45837,7 +45857,7 @@
         <v>0.5363</v>
       </c>
       <c r="M23" s="7">
-        <f t="shared" ref="M23:M24" si="2">L23/2.83168</f>
+        <f t="shared" ref="M23" si="2">L23/2.83168</f>
         <v>0.18939286925076279</v>
       </c>
       <c r="N23" t="s">
@@ -45930,10 +45950,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -46176,10 +46196,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -47434,10 +47454,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -48688,10 +48708,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -49942,10 +49962,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -50473,10 +50493,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -50662,10 +50682,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -51035,10 +51055,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -51502,10 +51522,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -51697,10 +51717,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -51942,10 +51962,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -52379,10 +52399,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -52962,10 +52982,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -53654,10 +53674,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -53911,8 +53931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5A00-000000000000}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53944,10 +53964,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -54469,7 +54489,7 @@
         <v>0.48399999999999999</v>
       </c>
       <c r="M13" s="8">
-        <f t="shared" ref="M12:M14" si="0">L13/2.83168</f>
+        <f t="shared" ref="M13:M14" si="0">L13/2.83168</f>
         <v>0.17092326816589445</v>
       </c>
       <c r="N13" t="s">
@@ -54561,10 +54581,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -55092,10 +55112,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -55331,10 +55351,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -55621,10 +55641,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -56040,10 +56060,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -56514,10 +56534,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -56988,10 +57008,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -57878,7 +57898,7 @@
         <v>1.243078313933778E-2</v>
       </c>
       <c r="N22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -57923,10 +57943,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Updated Dominion Energy rate with minor distribution charges (/bin/zsh.000055 / kWh)
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-rates/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CCE039-4FB6-6F44-9101-21D76B714782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B2DC8-728B-4D45-B6DD-590119A29EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17440" firstSheet="53" activeTab="64" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5691" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5787" uniqueCount="91">
   <si>
     <t>utility</t>
   </si>
@@ -3586,10 +3586,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="A1:O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3706,10 +3706,12 @@
         <v>4</v>
       </c>
       <c r="L3">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M3">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
@@ -3747,10 +3749,12 @@
         <v>4</v>
       </c>
       <c r="L4">
-        <v>3.8140000000000001E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="M4">
-        <v>3.8140000000000001E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
@@ -3788,10 +3792,12 @@
         <v>4</v>
       </c>
       <c r="L5">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M5">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N5" t="s">
         <v>14</v>
@@ -3829,10 +3835,12 @@
         <v>6</v>
       </c>
       <c r="L6">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M6">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N6" t="s">
         <v>14</v>
@@ -3870,10 +3878,12 @@
         <v>4</v>
       </c>
       <c r="L7">
-        <v>2.568E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="M7">
-        <v>2.568E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="N7" t="s">
         <v>14</v>
@@ -3911,10 +3921,12 @@
         <v>4</v>
       </c>
       <c r="L8">
-        <v>3.8140000000000001E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M8">
-        <v>3.8140000000000001E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N8" t="s">
         <v>14</v>
@@ -3952,10 +3964,12 @@
         <v>4</v>
       </c>
       <c r="L9">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M9">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N9" t="s">
         <v>14</v>
@@ -3993,10 +4007,12 @@
         <v>6</v>
       </c>
       <c r="L10">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M10">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N10" t="s">
         <v>14</v>
@@ -4034,10 +4050,12 @@
         <v>4</v>
       </c>
       <c r="L11">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M11">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N11" t="s">
         <v>14</v>
@@ -4075,10 +4093,12 @@
         <v>4</v>
       </c>
       <c r="L12">
-        <v>3.8140000000000001E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="M12">
-        <v>3.8140000000000001E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="N12" t="s">
         <v>14</v>
@@ -4116,10 +4136,12 @@
         <v>4</v>
       </c>
       <c r="L13">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M13">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N13" t="s">
         <v>14</v>
@@ -4157,10 +4179,12 @@
         <v>6</v>
       </c>
       <c r="L14">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M14">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N14" t="s">
         <v>14</v>
@@ -4201,10 +4225,12 @@
         <v>4</v>
       </c>
       <c r="L15">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M15">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N15" t="s">
         <v>17</v>
@@ -4245,12 +4271,12 @@
         <v>4</v>
       </c>
       <c r="L16">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="M16">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="N16" t="s">
         <v>17</v>
@@ -4291,10 +4317,12 @@
         <v>4</v>
       </c>
       <c r="L17">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M17">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N17" t="s">
         <v>17</v>
@@ -4335,10 +4363,12 @@
         <v>6</v>
       </c>
       <c r="L18">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M18">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N18" t="s">
         <v>17</v>
@@ -4379,10 +4409,12 @@
         <v>4</v>
       </c>
       <c r="L19">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M19">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N19" t="s">
         <v>17</v>
@@ -4423,12 +4455,12 @@
         <v>4</v>
       </c>
       <c r="L20">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="M20">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="N20" t="s">
         <v>17</v>
@@ -4469,10 +4501,12 @@
         <v>4</v>
       </c>
       <c r="L21">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M21">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N21" t="s">
         <v>17</v>
@@ -4513,10 +4547,12 @@
         <v>6</v>
       </c>
       <c r="L22">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M22">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N22" t="s">
         <v>17</v>
@@ -4557,10 +4593,12 @@
         <v>4</v>
       </c>
       <c r="L23">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M23">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N23" t="s">
         <v>17</v>
@@ -4601,12 +4639,12 @@
         <v>4</v>
       </c>
       <c r="L24">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="M24">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="N24" t="s">
         <v>17</v>
@@ -4647,10 +4685,12 @@
         <v>4</v>
       </c>
       <c r="L25">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M25">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N25" t="s">
         <v>17</v>
@@ -4691,12 +4731,566 @@
         <v>6</v>
       </c>
       <c r="L26">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M26">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>7</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M27">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28">
+        <v>5000</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <v>7</v>
+      </c>
+      <c r="I28">
+        <v>22</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="M28">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="N28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29">
+        <v>5000</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <v>22</v>
+      </c>
+      <c r="I29">
+        <v>24</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M29">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30">
+        <v>5000</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>24</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
+      </c>
+      <c r="K30">
+        <v>6</v>
+      </c>
+      <c r="L30">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M30">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31">
+        <v>5000</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>4</v>
+      </c>
+      <c r="L31">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M31">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32">
+        <v>5000</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>9</v>
+      </c>
+      <c r="H32">
+        <v>10</v>
+      </c>
+      <c r="I32">
+        <v>22</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="M32">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="N32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33">
+        <v>5000</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>22</v>
+      </c>
+      <c r="I33">
+        <v>24</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M33">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34">
+        <v>5000</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>24</v>
+      </c>
+      <c r="J34">
+        <v>5</v>
+      </c>
+      <c r="K34">
+        <v>6</v>
+      </c>
+      <c r="L34">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M34">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35">
+        <v>5000</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <v>12</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>7</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+      <c r="L35">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M35">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36">
+        <v>5000</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>10</v>
+      </c>
+      <c r="G36">
+        <v>12</v>
+      </c>
+      <c r="H36">
+        <v>7</v>
+      </c>
+      <c r="I36">
+        <v>22</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="M36">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="N36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37">
+        <v>5000</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="G37">
+        <v>12</v>
+      </c>
+      <c r="H37">
+        <v>22</v>
+      </c>
+      <c r="I37">
+        <v>24</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>4</v>
+      </c>
+      <c r="L37">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M37">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38">
+        <v>5000</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38">
+        <v>12</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>24</v>
+      </c>
+      <c r="J38">
+        <v>5</v>
+      </c>
+      <c r="K38">
+        <v>6</v>
+      </c>
+      <c r="L38">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M38">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N38" t="s">
         <v>17</v>
       </c>
     </row>
@@ -14119,10 +14713,10 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14239,10 +14833,12 @@
         <v>4</v>
       </c>
       <c r="L3">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M3">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
@@ -14280,10 +14876,12 @@
         <v>4</v>
       </c>
       <c r="L4">
-        <v>3.8140000000000001E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="M4">
-        <v>3.8140000000000001E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
@@ -14321,10 +14919,12 @@
         <v>4</v>
       </c>
       <c r="L5">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M5">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N5" t="s">
         <v>14</v>
@@ -14362,10 +14962,12 @@
         <v>6</v>
       </c>
       <c r="L6">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M6">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N6" t="s">
         <v>14</v>
@@ -14403,10 +15005,12 @@
         <v>4</v>
       </c>
       <c r="L7">
-        <v>2.568E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="M7">
-        <v>2.568E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="N7" t="s">
         <v>14</v>
@@ -14444,10 +15048,12 @@
         <v>4</v>
       </c>
       <c r="L8">
-        <v>3.8140000000000001E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M8">
-        <v>3.8140000000000001E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N8" t="s">
         <v>14</v>
@@ -14485,10 +15091,12 @@
         <v>4</v>
       </c>
       <c r="L9">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M9">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N9" t="s">
         <v>14</v>
@@ -14526,10 +15134,12 @@
         <v>6</v>
       </c>
       <c r="L10">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M10">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N10" t="s">
         <v>14</v>
@@ -14567,10 +15177,12 @@
         <v>4</v>
       </c>
       <c r="L11">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M11">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N11" t="s">
         <v>14</v>
@@ -14608,10 +15220,12 @@
         <v>4</v>
       </c>
       <c r="L12">
-        <v>3.8140000000000001E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="M12">
-        <v>3.8140000000000001E-3</v>
+        <f>0.003814+0.000055</f>
+        <v>3.869E-3</v>
       </c>
       <c r="N12" t="s">
         <v>14</v>
@@ -14649,10 +15263,12 @@
         <v>4</v>
       </c>
       <c r="L13">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M13">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N13" t="s">
         <v>14</v>
@@ -14690,10 +15306,12 @@
         <v>6</v>
       </c>
       <c r="L14">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="M14">
-        <v>2.568E-3</v>
+        <f>0.002568+0.000055</f>
+        <v>2.6229999999999999E-3</v>
       </c>
       <c r="N14" t="s">
         <v>14</v>
@@ -14734,10 +15352,12 @@
         <v>4</v>
       </c>
       <c r="L15">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M15">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N15" t="s">
         <v>17</v>
@@ -14778,12 +15398,12 @@
         <v>4</v>
       </c>
       <c r="L16">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="M16">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="N16" t="s">
         <v>17</v>
@@ -14824,10 +15444,12 @@
         <v>4</v>
       </c>
       <c r="L17">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M17">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N17" t="s">
         <v>17</v>
@@ -14868,10 +15490,12 @@
         <v>6</v>
       </c>
       <c r="L18">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M18">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N18" t="s">
         <v>17</v>
@@ -14912,10 +15536,12 @@
         <v>4</v>
       </c>
       <c r="L19">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M19">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N19" t="s">
         <v>17</v>
@@ -14956,12 +15582,12 @@
         <v>4</v>
       </c>
       <c r="L20">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="M20">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="N20" t="s">
         <v>17</v>
@@ -15002,10 +15628,12 @@
         <v>4</v>
       </c>
       <c r="L21">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M21">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N21" t="s">
         <v>17</v>
@@ -15046,10 +15674,12 @@
         <v>6</v>
       </c>
       <c r="L22">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M22">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N22" t="s">
         <v>17</v>
@@ -15090,10 +15720,12 @@
         <v>4</v>
       </c>
       <c r="L23">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M23">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N23" t="s">
         <v>17</v>
@@ -15134,12 +15766,12 @@
         <v>4</v>
       </c>
       <c r="L24">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="M24">
-        <f>10.537+2.371</f>
-        <v>12.908000000000001</v>
+        <f>10.537+2.371+0.94-0.397</f>
+        <v>13.451000000000001</v>
       </c>
       <c r="N24" t="s">
         <v>17</v>
@@ -15180,10 +15812,12 @@
         <v>4</v>
       </c>
       <c r="L25">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M25">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N25" t="s">
         <v>17</v>
@@ -15224,12 +15858,566 @@
         <v>6</v>
       </c>
       <c r="L26">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M26">
-        <v>0.59699999999999998</v>
+        <f>0.597+0.94-0.397</f>
+        <v>1.1399999999999999</v>
       </c>
       <c r="N26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27">
+        <v>5000</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>7</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M27">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28">
+        <v>5000</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28">
+        <v>7</v>
+      </c>
+      <c r="I28">
+        <v>22</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="M28">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="N28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29">
+        <v>5000</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <v>22</v>
+      </c>
+      <c r="I29">
+        <v>24</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M29">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30">
+        <v>5000</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>5</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>24</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
+      </c>
+      <c r="K30">
+        <v>6</v>
+      </c>
+      <c r="L30">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M30">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N30" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31">
+        <v>5000</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>4</v>
+      </c>
+      <c r="L31">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M31">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32">
+        <v>5000</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>9</v>
+      </c>
+      <c r="H32">
+        <v>10</v>
+      </c>
+      <c r="I32">
+        <v>22</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="M32">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="N32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33">
+        <v>5000</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>9</v>
+      </c>
+      <c r="H33">
+        <v>22</v>
+      </c>
+      <c r="I33">
+        <v>24</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M33">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34">
+        <v>5000</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>24</v>
+      </c>
+      <c r="J34">
+        <v>5</v>
+      </c>
+      <c r="K34">
+        <v>6</v>
+      </c>
+      <c r="L34">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M34">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35">
+        <v>5000</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <v>12</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>7</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+      <c r="L35">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M35">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36">
+        <v>5000</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>10</v>
+      </c>
+      <c r="G36">
+        <v>12</v>
+      </c>
+      <c r="H36">
+        <v>7</v>
+      </c>
+      <c r="I36">
+        <v>22</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="M36">
+        <f>10.537+2.371- 0.3+0.709</f>
+        <v>13.317</v>
+      </c>
+      <c r="N36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37">
+        <v>5000</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+      <c r="G37">
+        <v>12</v>
+      </c>
+      <c r="H37">
+        <v>22</v>
+      </c>
+      <c r="I37">
+        <v>24</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>4</v>
+      </c>
+      <c r="L37">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M37">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N37" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38">
+        <v>5000</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38">
+        <v>12</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>24</v>
+      </c>
+      <c r="J38">
+        <v>5</v>
+      </c>
+      <c r="K38">
+        <v>6</v>
+      </c>
+      <c r="L38">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="M38">
+        <f>0.597 - 0.3+0.709</f>
+        <v>1.006</v>
+      </c>
+      <c r="N38" t="s">
         <v>17</v>
       </c>
     </row>
@@ -33712,7 +34900,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35887,7 +37075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Ohio Edison and Xcel Energy (Colorado)
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B2DC8-728B-4D45-B6DD-590119A29EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFADA600-FD16-6746-9CB1-E6CCCEDAB409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="65" activeTab="76" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5787" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5799" uniqueCount="95">
   <si>
     <t>utility</t>
   </si>
@@ -405,6 +405,18 @@
   </si>
   <si>
     <t>basic_charge_limit (imperial)</t>
+  </si>
+  <si>
+    <t>Includes Delivery Capital Recovery Rider</t>
+  </si>
+  <si>
+    <t>Includes generation and fuel charges</t>
+  </si>
+  <si>
+    <t>Includes DSMCA, PCCA, and TCA</t>
+  </si>
+  <si>
+    <t>Includes Electricity Commodity Adjustment (ECA)</t>
   </si>
 </sst>
 </file>
@@ -3588,7 +3600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="A1:O38"/>
     </sheetView>
   </sheetViews>
@@ -3921,11 +3933,11 @@
         <v>4</v>
       </c>
       <c r="L8">
-        <f>0.002568+0.000055</f>
+        <f t="shared" ref="L8:M11" si="0">0.002568+0.000055</f>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="M8">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="N8" t="s">
@@ -3964,11 +3976,11 @@
         <v>4</v>
       </c>
       <c r="L9">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="M9">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="N9" t="s">
@@ -4007,11 +4019,11 @@
         <v>6</v>
       </c>
       <c r="L10">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="M10">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="N10" t="s">
@@ -4050,11 +4062,11 @@
         <v>4</v>
       </c>
       <c r="L11">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="M11">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="N11" t="s">
@@ -4317,11 +4329,11 @@
         <v>4</v>
       </c>
       <c r="L17">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" ref="L17:M19" si="1">0.597+0.94-0.397</f>
         <v>1.1399999999999999</v>
       </c>
       <c r="M17">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N17" t="s">
@@ -4363,11 +4375,11 @@
         <v>6</v>
       </c>
       <c r="L18">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="M18">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N18" t="s">
@@ -4409,11 +4421,11 @@
         <v>4</v>
       </c>
       <c r="L19">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="M19">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N19" t="s">
@@ -4501,11 +4513,11 @@
         <v>4</v>
       </c>
       <c r="L21">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" ref="L21:M23" si="2">0.597+0.94-0.397</f>
         <v>1.1399999999999999</v>
       </c>
       <c r="M21">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="2"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N21" t="s">
@@ -4547,11 +4559,11 @@
         <v>6</v>
       </c>
       <c r="L22">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="2"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="M22">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="2"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N22" t="s">
@@ -4593,11 +4605,11 @@
         <v>4</v>
       </c>
       <c r="L23">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="2"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="M23">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="2"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N23" t="s">
@@ -4869,11 +4881,11 @@
         <v>4</v>
       </c>
       <c r="L29">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" ref="L29:M31" si="3">0.597 - 0.3+0.709</f>
         <v>1.006</v>
       </c>
       <c r="M29">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="3"/>
         <v>1.006</v>
       </c>
       <c r="N29" t="s">
@@ -4915,11 +4927,11 @@
         <v>6</v>
       </c>
       <c r="L30">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="3"/>
         <v>1.006</v>
       </c>
       <c r="M30">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="3"/>
         <v>1.006</v>
       </c>
       <c r="N30" t="s">
@@ -4961,11 +4973,11 @@
         <v>4</v>
       </c>
       <c r="L31">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="3"/>
         <v>1.006</v>
       </c>
       <c r="M31">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="3"/>
         <v>1.006</v>
       </c>
       <c r="N31" t="s">
@@ -5053,11 +5065,11 @@
         <v>4</v>
       </c>
       <c r="L33">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" ref="L33:M35" si="4">0.597 - 0.3+0.709</f>
         <v>1.006</v>
       </c>
       <c r="M33">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="4"/>
         <v>1.006</v>
       </c>
       <c r="N33" t="s">
@@ -5099,11 +5111,11 @@
         <v>6</v>
       </c>
       <c r="L34">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="4"/>
         <v>1.006</v>
       </c>
       <c r="M34">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="4"/>
         <v>1.006</v>
       </c>
       <c r="N34" t="s">
@@ -5145,11 +5157,11 @@
         <v>4</v>
       </c>
       <c r="L35">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="4"/>
         <v>1.006</v>
       </c>
       <c r="M35">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="4"/>
         <v>1.006</v>
       </c>
       <c r="N35" t="s">
@@ -7898,7 +7910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
@@ -13083,7 +13095,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15048,11 +15060,11 @@
         <v>4</v>
       </c>
       <c r="L8">
-        <f>0.002568+0.000055</f>
+        <f t="shared" ref="L8:M11" si="0">0.002568+0.000055</f>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="M8">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="N8" t="s">
@@ -15091,11 +15103,11 @@
         <v>4</v>
       </c>
       <c r="L9">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="M9">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="N9" t="s">
@@ -15134,11 +15146,11 @@
         <v>6</v>
       </c>
       <c r="L10">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="M10">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="N10" t="s">
@@ -15177,11 +15189,11 @@
         <v>4</v>
       </c>
       <c r="L11">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="M11">
-        <f>0.002568+0.000055</f>
+        <f t="shared" si="0"/>
         <v>2.6229999999999999E-3</v>
       </c>
       <c r="N11" t="s">
@@ -15444,11 +15456,11 @@
         <v>4</v>
       </c>
       <c r="L17">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" ref="L17:M19" si="1">0.597+0.94-0.397</f>
         <v>1.1399999999999999</v>
       </c>
       <c r="M17">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N17" t="s">
@@ -15490,11 +15502,11 @@
         <v>6</v>
       </c>
       <c r="L18">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="M18">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N18" t="s">
@@ -15536,11 +15548,11 @@
         <v>4</v>
       </c>
       <c r="L19">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="M19">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="1"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N19" t="s">
@@ -15628,11 +15640,11 @@
         <v>4</v>
       </c>
       <c r="L21">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" ref="L21:M23" si="2">0.597+0.94-0.397</f>
         <v>1.1399999999999999</v>
       </c>
       <c r="M21">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="2"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N21" t="s">
@@ -15674,11 +15686,11 @@
         <v>6</v>
       </c>
       <c r="L22">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="2"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="M22">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="2"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N22" t="s">
@@ -15720,11 +15732,11 @@
         <v>4</v>
       </c>
       <c r="L23">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="2"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="M23">
-        <f>0.597+0.94-0.397</f>
+        <f t="shared" si="2"/>
         <v>1.1399999999999999</v>
       </c>
       <c r="N23" t="s">
@@ -15996,11 +16008,11 @@
         <v>4</v>
       </c>
       <c r="L29">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" ref="L29:M31" si="3">0.597 - 0.3+0.709</f>
         <v>1.006</v>
       </c>
       <c r="M29">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="3"/>
         <v>1.006</v>
       </c>
       <c r="N29" t="s">
@@ -16042,11 +16054,11 @@
         <v>6</v>
       </c>
       <c r="L30">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="3"/>
         <v>1.006</v>
       </c>
       <c r="M30">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="3"/>
         <v>1.006</v>
       </c>
       <c r="N30" t="s">
@@ -16088,11 +16100,11 @@
         <v>4</v>
       </c>
       <c r="L31">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="3"/>
         <v>1.006</v>
       </c>
       <c r="M31">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="3"/>
         <v>1.006</v>
       </c>
       <c r="N31" t="s">
@@ -16180,11 +16192,11 @@
         <v>4</v>
       </c>
       <c r="L33">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" ref="L33:M35" si="4">0.597 - 0.3+0.709</f>
         <v>1.006</v>
       </c>
       <c r="M33">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="4"/>
         <v>1.006</v>
       </c>
       <c r="N33" t="s">
@@ -16226,11 +16238,11 @@
         <v>6</v>
       </c>
       <c r="L34">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="4"/>
         <v>1.006</v>
       </c>
       <c r="M34">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="4"/>
         <v>1.006</v>
       </c>
       <c r="N34" t="s">
@@ -16272,11 +16284,11 @@
         <v>4</v>
       </c>
       <c r="L35">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="4"/>
         <v>1.006</v>
       </c>
       <c r="M35">
-        <f>0.597 - 0.3+0.709</f>
+        <f t="shared" si="4"/>
         <v>1.006</v>
       </c>
       <c r="N35" t="s">
@@ -17977,7 +17989,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18347,7 +18359,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18682,7 +18694,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18758,10 +18770,12 @@
         <v>11</v>
       </c>
       <c r="L2">
-        <v>150</v>
+        <f>150+238.878</f>
+        <v>388.87799999999999</v>
       </c>
       <c r="M2">
-        <v>150</v>
+        <f>150+238.878</f>
+        <v>388.87799999999999</v>
       </c>
       <c r="N2" t="s">
         <v>12</v>
@@ -18799,16 +18813,18 @@
         <v>6</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <f>0.003154+0.000447+0.0004+0.001623</f>
+        <v>5.6240000000000005E-3</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <f>0.003154+0.000447+0.0004+0.001623</f>
+        <v>5.6240000000000005E-3</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -18846,13 +18862,18 @@
         <v>6</v>
       </c>
       <c r="L4">
-        <v>2.2549999999999999</v>
+        <f>2.255+1.1102</f>
+        <v>3.3651999999999997</v>
       </c>
       <c r="M4">
-        <v>2.2549999999999999</v>
+        <f>2.255+1.1102</f>
+        <v>3.3651999999999997</v>
       </c>
       <c r="N4" t="s">
         <v>17</v>
+      </c>
+      <c r="O4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -31865,7 +31886,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:E2"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41797,7 +41818,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -45666,10 +45687,10 @@
 
 <file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4C00-000000000000}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -45777,33 +45798,35 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L3">
-        <v>4.5799999999999999E-3</v>
+        <f>0.02325+0.00458</f>
+        <v>2.7830000000000001E-2</v>
       </c>
       <c r="M3">
-        <v>4.5799999999999999E-3</v>
+        <f>0.02325+0.00458</f>
+        <v>2.7830000000000001E-2</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
       </c>
+      <c r="O3" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -45815,28 +45838,30 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="I4">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L4">
-        <v>9.5500000000000007</v>
+        <f>0.04069+0.00458</f>
+        <v>4.5269999999999998E-2</v>
       </c>
       <c r="M4">
-        <v>9.5500000000000007</v>
+        <f>0.04069+0.00458</f>
+        <v>4.5269999999999998E-2</v>
       </c>
       <c r="N4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -45844,10 +45869,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -45856,13 +45878,13 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G5">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="I5">
         <v>24</v>
@@ -45871,16 +45893,18 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L5">
-        <v>14.26</v>
+        <f>0.02325+0.00458</f>
+        <v>2.7830000000000001E-2</v>
       </c>
       <c r="M5">
-        <v>14.26</v>
+        <f>0.02325+0.00458</f>
+        <v>2.7830000000000001E-2</v>
       </c>
       <c r="N5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -45888,10 +45912,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -45900,7 +45921,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>12</v>
@@ -45912,19 +45933,21 @@
         <v>24</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K6">
         <v>6</v>
       </c>
       <c r="L6">
-        <v>9.5500000000000007</v>
+        <f>0.02325+0.00458</f>
+        <v>2.7830000000000001E-2</v>
       </c>
       <c r="M6">
-        <v>9.5500000000000007</v>
+        <f>0.02325+0.00458</f>
+        <v>2.7830000000000001E-2</v>
       </c>
       <c r="N6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -45935,7 +45958,7 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -45947,7 +45970,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -45962,10 +45985,10 @@
         <v>6</v>
       </c>
       <c r="L7">
-        <v>3.86</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="M7">
-        <v>3.86</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="N7" t="s">
         <v>17</v>
@@ -45973,27 +45996,57 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>24</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
       </c>
       <c r="L8">
-        <v>136.22</v>
+        <v>14.26</v>
       </c>
       <c r="M8">
-        <v>136.22</v>
+        <v>14.26</v>
       </c>
       <c r="N8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -46002,7 +46055,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>12</v>
@@ -46020,19 +46073,18 @@
         <v>6</v>
       </c>
       <c r="L9">
-        <v>2.759E-2</v>
-      </c>
-      <c r="M9" s="7">
-        <f t="shared" ref="M9:M10" si="0">L9/2.83168</f>
-        <v>9.7433325799525378E-3</v>
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="M9">
+        <v>9.5500000000000007</v>
       </c>
       <c r="N9" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -46065,13 +46117,121 @@
         <v>6</v>
       </c>
       <c r="L10">
+        <f>3.86+0.53+0.31+1.18</f>
+        <v>5.879999999999999</v>
+      </c>
+      <c r="M10">
+        <f>3.86+0.53+0.31+1.18</f>
+        <v>5.879999999999999</v>
+      </c>
+      <c r="N10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11">
+        <v>136.22</v>
+      </c>
+      <c r="M11">
+        <v>136.22</v>
+      </c>
+      <c r="N11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>24</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <v>2.759E-2</v>
+      </c>
+      <c r="M12" s="7">
+        <f t="shared" ref="M12:M13" si="0">L12/2.83168</f>
+        <v>9.7433325799525378E-3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>24</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="L13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M13" s="9">
         <f t="shared" si="0"/>
         <v>0.38846197310430558</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N13" t="s">
         <v>88</v>
       </c>
     </row>
@@ -59099,7 +59259,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added cost of fuel to We Energies rate
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFADA600-FD16-6746-9CB1-E6CCCEDAB409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06484720-1A07-0441-9B91-E6D03BE6CA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="65" activeTab="76" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17540" firstSheet="77" activeTab="88" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -45689,8 +45689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4C00-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -53714,8 +53714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5800-000000000000}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added FCA to OG&E
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C7499E-380D-ED41-9BA7-AE322B649469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049C5D3A-065A-724C-BB21-DCB35A6C74C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="39" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6096" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6100" uniqueCount="97">
   <si>
     <t>utility</t>
   </si>
@@ -420,6 +420,9 @@
   </si>
   <si>
     <t>Includes TVA Fuel Cost Adjustment</t>
+  </si>
+  <si>
+    <t>Includes Fuel Cost Adjustment (FCA) Factor</t>
   </si>
 </sst>
 </file>
@@ -5316,10 +5319,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5436,13 +5439,18 @@
         <v>6</v>
       </c>
       <c r="L3">
-        <v>3.0999999999999999E-3</v>
+        <f>0.0031+0.016834</f>
+        <v>1.9933999999999997E-2</v>
       </c>
       <c r="M3">
-        <v>3.0999999999999999E-3</v>
+        <f>0.0031+0.016834</f>
+        <v>1.9933999999999997E-2</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -5477,10 +5485,12 @@
         <v>4</v>
       </c>
       <c r="L4">
-        <v>3.0999999999999999E-3</v>
+        <f>0.0031+0.017962</f>
+        <v>2.1061999999999997E-2</v>
       </c>
       <c r="M4">
-        <v>3.0999999999999999E-3</v>
+        <f>0.0031+0.017962</f>
+        <v>2.1061999999999997E-2</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
@@ -5518,10 +5528,12 @@
         <v>4</v>
       </c>
       <c r="L5">
-        <v>4.4299999999999999E-2</v>
+        <f>0.0443+0.034226</f>
+        <v>7.8525999999999999E-2</v>
       </c>
       <c r="M5">
-        <v>4.4299999999999999E-2</v>
+        <f>0.0443+0.034226</f>
+        <v>7.8525999999999999E-2</v>
       </c>
       <c r="N5" t="s">
         <v>14</v>
@@ -5559,10 +5571,12 @@
         <v>4</v>
       </c>
       <c r="L6">
-        <v>3.0999999999999999E-3</v>
+        <f>0.0031+0.017962</f>
+        <v>2.1061999999999997E-2</v>
       </c>
       <c r="M6">
-        <v>3.0999999999999999E-3</v>
+        <f>0.0031+0.017962</f>
+        <v>2.1061999999999997E-2</v>
       </c>
       <c r="N6" t="s">
         <v>14</v>
@@ -5600,10 +5614,12 @@
         <v>6</v>
       </c>
       <c r="L7">
-        <v>3.0999999999999999E-3</v>
+        <f>0.0031+0.017962</f>
+        <v>2.1061999999999997E-2</v>
       </c>
       <c r="M7">
-        <v>3.0999999999999999E-3</v>
+        <f>0.0031+0.017962</f>
+        <v>2.1061999999999997E-2</v>
       </c>
       <c r="N7" t="s">
         <v>14</v>
@@ -5626,7 +5642,7 @@
         <v>10</v>
       </c>
       <c r="G8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -5641,10 +5657,12 @@
         <v>6</v>
       </c>
       <c r="L8">
-        <v>3.0999999999999999E-3</v>
+        <f>0.0031+0.022174</f>
+        <v>2.5273999999999998E-2</v>
       </c>
       <c r="M8">
-        <v>3.0999999999999999E-3</v>
+        <f>0.0031+0.022174</f>
+        <v>2.5273999999999998E-2</v>
       </c>
       <c r="N8" t="s">
         <v>14</v>
@@ -5655,42 +5673,85 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <f>0.0031+0.019452</f>
+        <v>2.2551999999999999E-2</v>
+      </c>
+      <c r="M9">
+        <f>0.0031+0.019452</f>
+        <v>2.2551999999999999E-2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>1</v>
       </c>
-      <c r="G9">
-        <v>12</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>24</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>6</v>
-      </c>
-      <c r="L9">
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>24</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
         <v>7.1280000000000001</v>
       </c>
-      <c r="M9">
+      <c r="M10">
         <v>7.1280000000000001</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N10" t="s">
         <v>17</v>
       </c>
     </row>
@@ -32135,8 +32196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added fuel cost recovery to Georgia Power
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049C5D3A-065A-724C-BB21-DCB35A6C74C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362C2A4C-A9AE-1C4B-AA03-1E475EB893AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="35" activeTab="46" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6100" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6143" uniqueCount="98">
   <si>
     <t>utility</t>
   </si>
@@ -423,6 +423,9 @@
   </si>
   <si>
     <t>Includes Fuel Cost Adjustment (FCA) Factor</t>
+  </si>
+  <si>
+    <t>Includes Fuel Cost Recovery Schedule: "FCR-25"</t>
   </si>
 </sst>
 </file>
@@ -5321,8 +5324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27493,10 +27496,10 @@
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27599,7 +27602,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -27614,13 +27617,18 @@
         <v>6</v>
       </c>
       <c r="L3">
-        <v>0.13490099999999999</v>
+        <f>0.134901+0.02471</f>
+        <v>0.159611</v>
       </c>
       <c r="M3">
-        <v>0.13490099999999999</v>
+        <f>0.134901+0.02471</f>
+        <v>0.159611</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -27640,7 +27648,7 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -27655,10 +27663,12 @@
         <v>6</v>
       </c>
       <c r="L4">
-        <v>0.12234</v>
+        <f>0.12234+0.02471</f>
+        <v>0.14705000000000001</v>
       </c>
       <c r="M4">
-        <v>0.12234</v>
+        <f>0.12234+0.02471</f>
+        <v>0.14705000000000001</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
@@ -27681,7 +27691,7 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -27696,10 +27706,12 @@
         <v>6</v>
       </c>
       <c r="L5">
-        <v>0.10434499999999999</v>
+        <f>0.104345+0.02471</f>
+        <v>0.129055</v>
       </c>
       <c r="M5">
-        <v>0.10434499999999999</v>
+        <f>0.104345+0.02471</f>
+        <v>0.129055</v>
       </c>
       <c r="N5" t="s">
         <v>14</v>
@@ -27722,7 +27734,7 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -27737,10 +27749,12 @@
         <v>6</v>
       </c>
       <c r="L6">
-        <v>8.0448000000000006E-2</v>
+        <f>0.080448+0.02471</f>
+        <v>0.105158</v>
       </c>
       <c r="M6">
-        <v>8.0448000000000006E-2</v>
+        <f>0.080448+0.02471</f>
+        <v>0.105158</v>
       </c>
       <c r="N6" t="s">
         <v>14</v>
@@ -27763,7 +27777,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -27778,10 +27792,12 @@
         <v>6</v>
       </c>
       <c r="L7">
-        <v>1.3858000000000001E-2</v>
+        <f>0.013858+0.02471</f>
+        <v>3.8567999999999998E-2</v>
       </c>
       <c r="M7">
-        <v>1.3858000000000001E-2</v>
+        <f>0.013858+0.02471</f>
+        <v>3.8567999999999998E-2</v>
       </c>
       <c r="N7" t="s">
         <v>14</v>
@@ -27804,7 +27820,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -27819,10 +27835,12 @@
         <v>6</v>
       </c>
       <c r="L8">
-        <v>1.0449E-2</v>
+        <f>0.010449+0.02471</f>
+        <v>3.5158999999999996E-2</v>
       </c>
       <c r="M8">
-        <v>1.0449E-2</v>
+        <f>0.010449+0.02471</f>
+        <v>3.5158999999999996E-2</v>
       </c>
       <c r="N8" t="s">
         <v>14</v>
@@ -27845,7 +27863,7 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -27860,10 +27878,12 @@
         <v>6</v>
       </c>
       <c r="L9">
-        <v>7.8410000000000007E-3</v>
+        <f>0.007841+0.02471</f>
+        <v>3.2550999999999997E-2</v>
       </c>
       <c r="M9">
-        <v>7.8410000000000007E-3</v>
+        <f>0.007841+0.02471</f>
+        <v>3.2550999999999997E-2</v>
       </c>
       <c r="N9" t="s">
         <v>14</v>
@@ -27875,10 +27895,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -27887,10 +27904,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G10">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -27905,71 +27922,676 @@
         <v>6</v>
       </c>
       <c r="L10">
-        <v>9.6999999999999993</v>
+        <f>0.134901+0.025022</f>
+        <v>0.15992299999999998</v>
       </c>
       <c r="M10">
-        <v>9.6999999999999993</v>
+        <f>0.134901+0.025022</f>
+        <v>0.15992299999999998</v>
       </c>
       <c r="N10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>3000</v>
+      </c>
+      <c r="E11">
+        <v>3000</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>24</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
       </c>
       <c r="L11">
-        <v>1263.96</v>
+        <f>0.12234+0.025022</f>
+        <v>0.14736199999999999</v>
       </c>
       <c r="M11">
-        <v>1263.96</v>
+        <f>0.12234+0.025022</f>
+        <v>0.14736199999999999</v>
       </c>
       <c r="N11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>10000</v>
+      </c>
+      <c r="E12">
+        <v>10000</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>24</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <f>0.104345+0.025022</f>
+        <v>0.12936699999999998</v>
+      </c>
+      <c r="M12">
+        <f>0.104345+0.025022</f>
+        <v>0.12936699999999998</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>200000</v>
+      </c>
+      <c r="E13">
+        <v>200000</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>24</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <f>0.080448+0.025022</f>
+        <v>0.10547000000000001</v>
+      </c>
+      <c r="M13">
+        <f>0.080448+0.025022</f>
+        <v>0.10547000000000001</v>
+      </c>
+      <c r="N13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1276333.33333333</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1276333.33333333</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>9</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>24</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <f>0.013858+0.025022</f>
+        <v>3.8879999999999998E-2</v>
+      </c>
+      <c r="M14">
+        <f>0.013858+0.025022</f>
+        <v>3.8879999999999998E-2</v>
+      </c>
+      <c r="N14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="10">
+        <v>2552666.6666666698</v>
+      </c>
+      <c r="E15" s="10">
+        <v>2552666.6666666698</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>24</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>6</v>
+      </c>
+      <c r="L15">
+        <f>0.010449+0.025022</f>
+        <v>3.5471000000000003E-2</v>
+      </c>
+      <c r="M15">
+        <f>0.010449+0.025022</f>
+        <v>3.5471000000000003E-2</v>
+      </c>
+      <c r="N15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>3829000</v>
+      </c>
+      <c r="E16">
+        <v>3829000</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>24</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <f>0.007841+0.025022</f>
+        <v>3.2863000000000003E-2</v>
+      </c>
+      <c r="M16">
+        <f>0.007841+0.025022</f>
+        <v>3.2863000000000003E-2</v>
+      </c>
+      <c r="N16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="G17">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>24</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>6</v>
+      </c>
+      <c r="L17">
+        <f>0.134901+0.02471</f>
+        <v>0.159611</v>
+      </c>
+      <c r="M17">
+        <f>0.134901+0.02471</f>
+        <v>0.159611</v>
+      </c>
+      <c r="N17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>3000</v>
+      </c>
+      <c r="E18">
+        <v>3000</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>12</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>24</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>6</v>
+      </c>
+      <c r="L18">
+        <f>0.12234+0.02471</f>
+        <v>0.14705000000000001</v>
+      </c>
+      <c r="M18">
+        <f>0.12234+0.02471</f>
+        <v>0.14705000000000001</v>
+      </c>
+      <c r="N18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>10000</v>
+      </c>
+      <c r="E19">
+        <v>10000</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>12</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>24</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>6</v>
+      </c>
+      <c r="L19">
+        <f>0.104345+0.02471</f>
+        <v>0.129055</v>
+      </c>
+      <c r="M19">
+        <f>0.104345+0.02471</f>
+        <v>0.129055</v>
+      </c>
+      <c r="N19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>200000</v>
+      </c>
+      <c r="E20">
+        <v>200000</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+      <c r="G20">
+        <v>12</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>24</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>6</v>
+      </c>
+      <c r="L20">
+        <f>0.080448+0.02471</f>
+        <v>0.105158</v>
+      </c>
+      <c r="M20">
+        <f>0.080448+0.02471</f>
+        <v>0.105158</v>
+      </c>
+      <c r="N20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1276333.33333333</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1276333.33333333</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>12</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>24</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>6</v>
+      </c>
+      <c r="L21">
+        <f>0.013858+0.02471</f>
+        <v>3.8567999999999998E-2</v>
+      </c>
+      <c r="M21">
+        <f>0.013858+0.02471</f>
+        <v>3.8567999999999998E-2</v>
+      </c>
+      <c r="N21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="10">
+        <v>2552666.6666666698</v>
+      </c>
+      <c r="E22" s="10">
+        <v>2552666.6666666698</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22">
+        <v>12</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>24</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+      <c r="L22">
+        <f>0.010449+0.02471</f>
+        <v>3.5158999999999996E-2</v>
+      </c>
+      <c r="M22">
+        <f>0.010449+0.02471</f>
+        <v>3.5158999999999996E-2</v>
+      </c>
+      <c r="N22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>3829000</v>
+      </c>
+      <c r="E23">
+        <v>3829000</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <v>12</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>24</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>6</v>
+      </c>
+      <c r="L23">
+        <f>0.007841+0.02471</f>
+        <v>3.2550999999999997E-2</v>
+      </c>
+      <c r="M23">
+        <f>0.007841+0.02471</f>
+        <v>3.2550999999999997E-2</v>
+      </c>
+      <c r="N23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>24</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>6</v>
+      </c>
+      <c r="L24">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="M24">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="N24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25">
+        <v>1263.96</v>
+      </c>
+      <c r="M25">
+        <v>1263.96</v>
+      </c>
+      <c r="N25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
         <v>1</v>
       </c>
-      <c r="G12">
-        <v>12</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>24</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>6</v>
-      </c>
-      <c r="L12">
+      <c r="G26">
+        <v>12</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>24</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>6</v>
+      </c>
+      <c r="L26">
         <v>1.1292</v>
       </c>
-      <c r="M12" s="6">
-        <f>L12/2.83168</f>
+      <c r="M26" s="6">
+        <f>L26/2.83168</f>
         <v>0.39877387275398352</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N26" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>

<commit_message>
switched Ohio Edison to TOU rates
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60BA4C0-579E-A04A-B334-6D1EB4B441D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DA548C-B6C3-1C45-8300-84032B406A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="30" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="31" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6373" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6416" uniqueCount="100">
   <si>
     <t>utility</t>
   </si>
@@ -404,9 +404,6 @@
     <t>Includes Delivery Capital Recovery Rider</t>
   </si>
   <si>
-    <t>Includes generation and fuel charges</t>
-  </si>
-  <si>
     <t>Includes DSMCA, PCCA, and TCA</t>
   </si>
   <si>
@@ -429,6 +426,12 @@
   </si>
   <si>
     <t>Includes delivery and generation service</t>
+  </si>
+  <si>
+    <t>Includes Riders GCR, TSA, GEN, and Fuel</t>
+  </si>
+  <si>
+    <t>Time-of-day option selected for Rider GEN</t>
   </si>
 </sst>
 </file>
@@ -2890,7 +2893,7 @@
         <v>17</v>
       </c>
       <c r="O3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -2937,7 +2940,7 @@
         <v>17</v>
       </c>
       <c r="O4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -3071,7 +3074,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -6085,7 +6088,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -11615,7 +11618,7 @@
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -21047,10 +21050,10 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21154,13 +21157,13 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -21169,18 +21172,18 @@
         <v>6</v>
       </c>
       <c r="L3">
-        <f>0.003154+0.000447+0.0004+0.001623</f>
-        <v>5.6240000000000005E-3</v>
+        <f>0.003154+0.000447+0.001623+0.013815+0.024284</f>
+        <v>4.3323E-2</v>
       </c>
       <c r="M3">
-        <f>0.003154+0.000447+0.0004+0.001623</f>
-        <v>5.6240000000000005E-3</v>
+        <f>0.003154+0.000447+0.001623+0.013815+0.024284</f>
+        <v>4.3323E-2</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -21188,10 +21191,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -21203,13 +21203,13 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I4">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -21218,170 +21218,778 @@
         <v>6</v>
       </c>
       <c r="L4">
+        <f>0.003154+0.000447+0.001623+0.013815+0.037215</f>
+        <v>5.6253999999999998E-2</v>
+      </c>
+      <c r="M4">
+        <f>0.003154+0.000447+0.001623+0.013815+0.037215</f>
+        <v>5.6253999999999998E-2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>18</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <f>0.003154+0.000447+0.001623+0.013815+0.048567</f>
+        <v>6.7605999999999999E-2</v>
+      </c>
+      <c r="M5">
+        <f>0.003154+0.000447+0.001623+0.013815+0.048567</f>
+        <v>6.7605999999999999E-2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
+      <c r="I6">
+        <v>22</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>6</v>
+      </c>
+      <c r="L6">
+        <f>0.003154+0.000447+0.001623+0.013815+0.037215</f>
+        <v>5.6253999999999998E-2</v>
+      </c>
+      <c r="M6">
+        <f>0.003154+0.000447+0.001623+0.013815+0.037215</f>
+        <v>5.6253999999999998E-2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>22</v>
+      </c>
+      <c r="I7">
+        <v>24</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <f>0.003154+0.000447+0.001623+0.013815+0.024284</f>
+        <v>4.3323E-2</v>
+      </c>
+      <c r="M7">
+        <f>0.003154+0.000447+0.001623+0.013815+0.024284</f>
+        <v>4.3323E-2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <f>0.003154+0.000447+0.001623+0.013815+0.031373</f>
+        <v>5.0411999999999998E-2</v>
+      </c>
+      <c r="M8">
+        <f>0.003154+0.000447+0.001623+0.013815+0.031373</f>
+        <v>5.0411999999999998E-2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <f>0.003154+0.000447+0.001623+0.013815+0.040864</f>
+        <v>5.9902999999999998E-2</v>
+      </c>
+      <c r="M9">
+        <f>0.003154+0.000447+0.001623+0.013815+0.040864</f>
+        <v>5.9902999999999998E-2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>12</v>
+      </c>
+      <c r="I10">
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <f>0.003154+0.000447+0.001623+0.013815+0.062747</f>
+        <v>8.1785999999999998E-2</v>
+      </c>
+      <c r="M10">
+        <f>0.003154+0.000447+0.001623+0.013815+0.062747</f>
+        <v>8.1785999999999998E-2</v>
+      </c>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>18</v>
+      </c>
+      <c r="I11">
+        <v>22</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <f>0.003154+0.000447+0.001623+0.013815+0.040864</f>
+        <v>5.9902999999999998E-2</v>
+      </c>
+      <c r="M11">
+        <f>0.003154+0.000447+0.001623+0.013815+0.040864</f>
+        <v>5.9902999999999998E-2</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>22</v>
+      </c>
+      <c r="I12">
+        <v>24</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <f>0.003154+0.000447+0.001623+0.013815+0.031373</f>
+        <v>5.0411999999999998E-2</v>
+      </c>
+      <c r="M12">
+        <f>0.003154+0.000447+0.001623+0.013815+0.031373</f>
+        <v>5.0411999999999998E-2</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <f>0.003154+0.000447+0.001623+0.013815+0.024284</f>
+        <v>4.3323E-2</v>
+      </c>
+      <c r="M13">
+        <f>0.003154+0.000447+0.001623+0.013815+0.024284</f>
+        <v>4.3323E-2</v>
+      </c>
+      <c r="N13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>12</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <f>0.003154+0.000447+0.001623+0.013815+0.037215</f>
+        <v>5.6253999999999998E-2</v>
+      </c>
+      <c r="M14">
+        <f>0.003154+0.000447+0.001623+0.013815+0.037215</f>
+        <v>5.6253999999999998E-2</v>
+      </c>
+      <c r="N14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>12</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <v>18</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>6</v>
+      </c>
+      <c r="L15">
+        <f>0.003154+0.000447+0.001623+0.013815+0.048567</f>
+        <v>6.7605999999999999E-2</v>
+      </c>
+      <c r="M15">
+        <f>0.003154+0.000447+0.001623+0.013815+0.048567</f>
+        <v>6.7605999999999999E-2</v>
+      </c>
+      <c r="N15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>12</v>
+      </c>
+      <c r="H16">
+        <v>18</v>
+      </c>
+      <c r="I16">
+        <v>22</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <f>0.003154+0.000447+0.001623+0.013815+0.037215</f>
+        <v>5.6253999999999998E-2</v>
+      </c>
+      <c r="M16">
+        <f>0.003154+0.000447+0.001623+0.013815+0.037215</f>
+        <v>5.6253999999999998E-2</v>
+      </c>
+      <c r="N16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>22</v>
+      </c>
+      <c r="I17">
+        <v>24</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>6</v>
+      </c>
+      <c r="L17">
+        <f>0.003154+0.000447+0.001623+0.013815+0.024284</f>
+        <v>4.3323E-2</v>
+      </c>
+      <c r="M17">
+        <f>0.003154+0.000447+0.001623+0.013815+0.024284</f>
+        <v>4.3323E-2</v>
+      </c>
+      <c r="N17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>12</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>24</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>6</v>
+      </c>
+      <c r="L18">
         <f>2.255+1.1102</f>
         <v>3.3651999999999997</v>
       </c>
-      <c r="M4">
+      <c r="M18">
         <f>2.255+1.1102</f>
         <v>3.3651999999999997</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N18" t="s">
         <v>17</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O18" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B19" t="s">
         <v>11</v>
       </c>
-      <c r="L5">
+      <c r="L19">
         <v>60</v>
       </c>
-      <c r="M5">
+      <c r="M19">
         <v>60</v>
       </c>
-      <c r="N5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="N19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
         <v>1</v>
       </c>
-      <c r="G6">
-        <v>12</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>24</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>6</v>
-      </c>
-      <c r="L6">
+      <c r="G20">
+        <v>12</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>24</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>6</v>
+      </c>
+      <c r="L20">
         <f>(1.25+5.597)/10.37</f>
         <v>0.66027000964320159</v>
       </c>
-      <c r="M6" s="6">
-        <f>L6/2.83168</f>
+      <c r="M20" s="6">
+        <f>L20/2.83168</f>
         <v>0.23317253702508814</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N20" t="s">
         <v>85</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O20" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21">
         <f>100*10.37</f>
         <v>1037</v>
       </c>
-      <c r="E7" s="10">
-        <f>D7*2.83168</f>
+      <c r="E21" s="10">
+        <f>D21*2.83168</f>
         <v>2936.4521599999998</v>
       </c>
-      <c r="F7">
+      <c r="F21">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>24</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>6</v>
-      </c>
-      <c r="L7">
+      <c r="G21">
+        <v>12</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>24</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>6</v>
+      </c>
+      <c r="L21">
         <f>(0.97+5.597)/10.37</f>
         <v>0.63326904532304729</v>
       </c>
-      <c r="M7" s="6">
-        <f>L7/2.83168</f>
+      <c r="M21" s="6">
+        <f>L21/2.83168</f>
         <v>0.22363722077460987</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22">
         <f>500*10.37</f>
         <v>5185</v>
       </c>
-      <c r="E8" s="10">
-        <f>D8*2.83168</f>
+      <c r="E22" s="10">
+        <f>D22*2.83168</f>
         <v>14682.2608</v>
       </c>
-      <c r="F8">
+      <c r="F22">
         <v>1</v>
       </c>
-      <c r="G8">
-        <v>12</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>24</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>6</v>
-      </c>
-      <c r="L8">
+      <c r="G22">
+        <v>12</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>24</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+      <c r="L22">
         <f>(0.82+5.597)/10.37</f>
         <v>0.61880424300867898</v>
       </c>
-      <c r="M8" s="6">
-        <f>L8/2.83168</f>
+      <c r="M22" s="6">
+        <f>L22/2.83168</f>
         <v>0.21852901564042512</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N22" t="s">
         <v>85</v>
       </c>
     </row>
@@ -26434,8 +27042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26458,7 +27066,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>22</v>
@@ -26567,7 +27175,7 @@
         <v>17</v>
       </c>
       <c r="O3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -26614,7 +27222,7 @@
         <v>17</v>
       </c>
       <c r="O4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -26748,7 +27356,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -28859,7 +29467,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -29971,7 +30579,7 @@
         <v>17</v>
       </c>
       <c r="O3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -30018,7 +30626,7 @@
         <v>17</v>
       </c>
       <c r="O4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -30152,7 +30760,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -32318,7 +32926,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -34658,7 +35266,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -51825,7 +52433,7 @@
         <v>17</v>
       </c>
       <c r="O3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -51872,7 +52480,7 @@
         <v>17</v>
       </c>
       <c r="O4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -52006,7 +52614,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -52961,7 +53569,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -53271,7 +53879,7 @@
         <v>17</v>
       </c>
       <c r="O10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -64651,7 +65259,7 @@
         <v>17</v>
       </c>
       <c r="O3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -64698,7 +65306,7 @@
         <v>17</v>
       </c>
       <c r="O4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -64832,7 +65440,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -65604,7 +66212,7 @@
         <v>17</v>
       </c>
       <c r="O3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -65651,7 +66259,7 @@
         <v>17</v>
       </c>
       <c r="O4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -65785,7 +66393,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Removing erroneous gas charges from two SCE facilities
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DA548C-B6C3-1C45-8300-84032B406A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E838637B-C0AC-C948-B56D-89C5563B9788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="31" activeTab="34" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="30" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6416" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6390" uniqueCount="100">
   <si>
     <t>utility</t>
   </si>
@@ -2758,10 +2758,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="A1:O22"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3464,7 +3464,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -3548,160 +3548,6 @@
       </c>
       <c r="N18" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="L19">
-        <f>0.49315*30</f>
-        <v>14.794499999999999</v>
-      </c>
-      <c r="M19">
-        <f>0.49315*30</f>
-        <v>14.794499999999999</v>
-      </c>
-      <c r="N19" t="s">
-        <v>12</v>
-      </c>
-      <c r="O19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f>D20*2.83168</f>
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>12</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>24</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>6</v>
-      </c>
-      <c r="L20">
-        <v>1.6166199999999999</v>
-      </c>
-      <c r="M20" s="6">
-        <f>L20/2.83168</f>
-        <v>0.57090490450898401</v>
-      </c>
-      <c r="N20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21">
-        <v>250</v>
-      </c>
-      <c r="E21">
-        <f>D21*2.83168</f>
-        <v>707.92</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>12</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>24</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>6</v>
-      </c>
-      <c r="L21">
-        <v>1.1773100000000001</v>
-      </c>
-      <c r="M21" s="6">
-        <f>L21/2.83168</f>
-        <v>0.41576378686857274</v>
-      </c>
-      <c r="N21" t="s">
-        <v>85</v>
-      </c>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22">
-        <v>4167</v>
-      </c>
-      <c r="E22" s="10">
-        <f>D22*2.83168</f>
-        <v>11799.610559999999</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>12</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>24</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>6</v>
-      </c>
-      <c r="L22">
-        <v>0.88275999999999999</v>
-      </c>
-      <c r="M22" s="6">
-        <f>L22/2.83168</f>
-        <v>0.31174426488868801</v>
-      </c>
-      <c r="N22" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -21052,8 +20898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:P22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27040,10 +26886,10 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27746,7 +27592,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -27789,7 +27635,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -27830,160 +27676,6 @@
       </c>
       <c r="N18" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="L19">
-        <f>0.49315*30</f>
-        <v>14.794499999999999</v>
-      </c>
-      <c r="M19">
-        <f>0.49315*30</f>
-        <v>14.794499999999999</v>
-      </c>
-      <c r="N19" t="s">
-        <v>12</v>
-      </c>
-      <c r="O19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f>D20*2.83168</f>
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>12</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>24</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>6</v>
-      </c>
-      <c r="L20">
-        <v>1.6166199999999999</v>
-      </c>
-      <c r="M20" s="6">
-        <f>L20/2.83168</f>
-        <v>0.57090490450898401</v>
-      </c>
-      <c r="N20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21">
-        <v>250</v>
-      </c>
-      <c r="E21">
-        <f>D21*2.83168</f>
-        <v>707.92</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>12</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>24</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>6</v>
-      </c>
-      <c r="L21">
-        <v>1.1773100000000001</v>
-      </c>
-      <c r="M21" s="6">
-        <f>L21/2.83168</f>
-        <v>0.41576378686857274</v>
-      </c>
-      <c r="N21" t="s">
-        <v>85</v>
-      </c>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22">
-        <v>4167</v>
-      </c>
-      <c r="E22" s="10">
-        <f>D22*2.83168</f>
-        <v>11799.610559999999</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>12</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>24</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>6</v>
-      </c>
-      <c r="L22">
-        <v>0.88275999999999999</v>
-      </c>
-      <c r="M22" s="6">
-        <f>L22/2.83168</f>
-        <v>0.31174426488868801</v>
-      </c>
-      <c r="N22" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added minor charges to TECO
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E838637B-C0AC-C948-B56D-89C5563B9788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C16329C-E69E-D54F-AA3A-0182A0F91211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="30" activeTab="41" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6390" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6391" uniqueCount="101">
   <si>
     <t>utility</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>Time-of-day option selected for Rider GEN</t>
+  </si>
+  <si>
+    <t>Includes fuel cost and environmental charge</t>
   </si>
 </sst>
 </file>
@@ -850,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -968,15 +971,18 @@
         <v>4</v>
       </c>
       <c r="L3">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="M3">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -1011,12 +1017,12 @@
         <v>4</v>
       </c>
       <c r="L4">
-        <f>0.0291+0.0462</f>
-        <v>7.5300000000000006E-2</v>
+        <f>0.02908+0.0462+0.00265</f>
+        <v>7.7929999999999999E-2</v>
       </c>
       <c r="M4">
-        <f>0.0291+0.0462</f>
-        <v>7.5300000000000006E-2</v>
+        <f>0.02908+0.0462+0.00265</f>
+        <v>7.7929999999999999E-2</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
@@ -1054,12 +1060,12 @@
         <v>4</v>
       </c>
       <c r="L5">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="M5">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="N5" t="s">
         <v>14</v>
@@ -1097,12 +1103,12 @@
         <v>4</v>
       </c>
       <c r="L6">
-        <f>0.0291+0.0462</f>
-        <v>7.5300000000000006E-2</v>
+        <f>0.02908+0.0462+0.00265</f>
+        <v>7.7929999999999999E-2</v>
       </c>
       <c r="M6">
-        <f>0.0291+0.0462</f>
-        <v>7.5300000000000006E-2</v>
+        <f>0.02908+0.0462+0.00265</f>
+        <v>7.7929999999999999E-2</v>
       </c>
       <c r="N6" t="s">
         <v>14</v>
@@ -1140,12 +1146,12 @@
         <v>4</v>
       </c>
       <c r="L7">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="M7">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="N7" t="s">
         <v>14</v>
@@ -1183,12 +1189,12 @@
         <v>4</v>
       </c>
       <c r="L8">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="M8">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="N8" t="s">
         <v>14</v>
@@ -1226,12 +1232,12 @@
         <v>4</v>
       </c>
       <c r="L9">
-        <f>0.0291+0.0462</f>
-        <v>7.5300000000000006E-2</v>
+        <f>0.02908+0.0462+0.00265</f>
+        <v>7.7929999999999999E-2</v>
       </c>
       <c r="M9">
-        <f>0.0291+0.0462</f>
-        <v>7.5300000000000006E-2</v>
+        <f>0.02908+0.0462+0.00265</f>
+        <v>7.7929999999999999E-2</v>
       </c>
       <c r="N9" t="s">
         <v>14</v>
@@ -1269,12 +1275,12 @@
         <v>4</v>
       </c>
       <c r="L10">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="M10">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="N10" t="s">
         <v>14</v>
@@ -1312,12 +1318,12 @@
         <v>4</v>
       </c>
       <c r="L11">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="M11">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="N11" t="s">
         <v>14</v>
@@ -1355,12 +1361,12 @@
         <v>4</v>
       </c>
       <c r="L12">
-        <f>0.0291+0.0462</f>
-        <v>7.5300000000000006E-2</v>
+        <f>0.02908+0.0462+0.00265</f>
+        <v>7.7929999999999999E-2</v>
       </c>
       <c r="M12">
-        <f>0.0291+0.0462</f>
-        <v>7.5300000000000006E-2</v>
+        <f>0.02908+0.0462+0.00265</f>
+        <v>7.7929999999999999E-2</v>
       </c>
       <c r="N12" t="s">
         <v>14</v>
@@ -1398,12 +1404,12 @@
         <v>4</v>
       </c>
       <c r="L13">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="M13">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="N13" t="s">
         <v>14</v>
@@ -1441,12 +1447,12 @@
         <v>4</v>
       </c>
       <c r="L14">
-        <f>0.0291+0.0462</f>
-        <v>7.5300000000000006E-2</v>
+        <f>0.02908+0.0462+0.00265</f>
+        <v>7.7929999999999999E-2</v>
       </c>
       <c r="M14">
-        <f>0.0291+0.0462</f>
-        <v>7.5300000000000006E-2</v>
+        <f>0.02908+0.0462+0.00265</f>
+        <v>7.7929999999999999E-2</v>
       </c>
       <c r="N14" t="s">
         <v>14</v>
@@ -1484,12 +1490,12 @@
         <v>4</v>
       </c>
       <c r="L15">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="M15">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="N15" t="s">
         <v>14</v>
@@ -1527,12 +1533,12 @@
         <v>6</v>
       </c>
       <c r="L16">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="M16">
-        <f>0.0105+0.041</f>
-        <v>5.1500000000000004E-2</v>
+        <f>0.01049+0.04099+0.00265</f>
+        <v>5.4129999999999998E-2</v>
       </c>
       <c r="N16" t="s">
         <v>14</v>
@@ -1793,10 +1799,12 @@
         <v>6</v>
       </c>
       <c r="L22">
-        <v>3.49</v>
+        <f>3.49+0.6+0.52+0.72</f>
+        <v>5.3299999999999992</v>
       </c>
       <c r="M22">
-        <v>3.49</v>
+        <f>3.49+0.6+0.52+0.72</f>
+        <v>5.3299999999999992</v>
       </c>
       <c r="N22" t="s">
         <v>17</v>
@@ -26888,7 +26896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added supply charge to Eversource (CT)
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C16329C-E69E-D54F-AA3A-0182A0F91211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C043E610-3372-3346-8EA6-10DEEBF39345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6391" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6525" uniqueCount="102">
   <si>
     <t>utility</t>
   </si>
@@ -435,6 +435,9 @@
   </si>
   <si>
     <t>Includes fuel cost and environmental charge</t>
+  </si>
+  <si>
+    <t>Includes generation supply and distribution service</t>
   </si>
 </sst>
 </file>
@@ -853,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41037,10 +41040,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27:M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41142,7 +41145,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -41157,13 +41160,18 @@
         <v>4</v>
       </c>
       <c r="L3">
-        <v>6.2199999999999998E-3</v>
+        <f>0.00622+0.10434</f>
+        <v>0.11056000000000001</v>
       </c>
       <c r="M3">
-        <v>6.2199999999999998E-3</v>
+        <f>0.00622+0.10434</f>
+        <v>0.11056000000000001</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -41183,7 +41191,7 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>12</v>
@@ -41198,16 +41206,15 @@
         <v>4</v>
       </c>
       <c r="L4">
-        <v>2.9080000000000002E-2</v>
+        <f>0.02908+0.10846</f>
+        <v>0.13754</v>
       </c>
       <c r="M4">
-        <v>2.9080000000000002E-2</v>
+        <f>0.02908+0.10846</f>
+        <v>0.13754</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
-      </c>
-      <c r="O4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -41227,7 +41234,7 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>20</v>
@@ -41242,10 +41249,12 @@
         <v>4</v>
       </c>
       <c r="L5">
-        <v>6.2199999999999998E-3</v>
+        <f>0.00622+0.10434</f>
+        <v>0.11056000000000001</v>
       </c>
       <c r="M5">
-        <v>6.2199999999999998E-3</v>
+        <f>0.00622+0.10434</f>
+        <v>0.11056000000000001</v>
       </c>
       <c r="N5" t="s">
         <v>14</v>
@@ -41268,7 +41277,7 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -41283,10 +41292,12 @@
         <v>6</v>
       </c>
       <c r="L6">
-        <v>6.2199999999999998E-3</v>
+        <f>0.00622+0.10434</f>
+        <v>0.11056000000000001</v>
       </c>
       <c r="M6">
-        <v>6.2199999999999998E-3</v>
+        <f>0.00622+0.10434</f>
+        <v>0.11056000000000001</v>
       </c>
       <c r="N6" t="s">
         <v>14</v>
@@ -41297,54 +41308,1947 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <f>0.00622+0.10308</f>
+        <v>0.10930000000000001</v>
+      </c>
+      <c r="M7">
+        <f>0.00622+0.10308</f>
+        <v>0.10930000000000001</v>
+      </c>
+      <c r="N7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <f>0.02908+0.10544</f>
+        <v>0.13452</v>
+      </c>
+      <c r="M8">
+        <f>0.02908+0.10544</f>
+        <v>0.13452</v>
+      </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9">
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <f>0.00622+0.10308</f>
+        <v>0.10930000000000001</v>
+      </c>
+      <c r="M9">
+        <f>0.00622+0.10308</f>
+        <v>0.10930000000000001</v>
+      </c>
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>24</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>6</v>
+      </c>
+      <c r="L10">
+        <f>0.00622+0.10308</f>
+        <v>0.10930000000000001</v>
+      </c>
+      <c r="M10">
+        <f>0.00622+0.10308</f>
+        <v>0.10930000000000001</v>
+      </c>
+      <c r="N10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>12</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <f>0.00622+0.08725</f>
+        <v>9.3469999999999998E-2</v>
+      </c>
+      <c r="M11">
+        <f>0.00622+0.08725</f>
+        <v>9.3469999999999998E-2</v>
+      </c>
+      <c r="N11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>20</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <f>0.02908+0.08588</f>
+        <v>0.11496000000000001</v>
+      </c>
+      <c r="M12">
+        <f>0.02908+0.08588</f>
+        <v>0.11496000000000001</v>
+      </c>
+      <c r="N12" t="s">
+        <v>14</v>
+      </c>
+      <c r="O12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>20</v>
+      </c>
+      <c r="I13">
+        <v>24</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <f>0.00622+0.08725</f>
+        <v>9.3469999999999998E-2</v>
+      </c>
+      <c r="M13">
+        <f>0.00622+0.08725</f>
+        <v>9.3469999999999998E-2</v>
+      </c>
+      <c r="N13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>24</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <f>0.00622+0.08725</f>
+        <v>9.3469999999999998E-2</v>
+      </c>
+      <c r="M14">
+        <f>0.00622+0.08725</f>
+        <v>9.3469999999999998E-2</v>
+      </c>
+      <c r="N14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <f>0.00622+0.0725</f>
+        <v>7.8719999999999998E-2</v>
+      </c>
+      <c r="M15">
+        <f>0.00622+0.0725</f>
+        <v>7.8719999999999998E-2</v>
+      </c>
+      <c r="N15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>12</v>
+      </c>
+      <c r="I16">
+        <v>20</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <f>0.02908+0.06478</f>
+        <v>9.3859999999999999E-2</v>
+      </c>
+      <c r="M16">
+        <f>0.02908+0.06478</f>
+        <v>9.3859999999999999E-2</v>
+      </c>
+      <c r="N16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
+      <c r="I17">
+        <v>24</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17">
+        <f>0.00622+0.0725</f>
+        <v>7.8719999999999998E-2</v>
+      </c>
+      <c r="M17">
+        <f>0.00622+0.0725</f>
+        <v>7.8719999999999998E-2</v>
+      </c>
+      <c r="N17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>24</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>6</v>
+      </c>
+      <c r="L18">
+        <f>0.00622+0.0725</f>
+        <v>7.8719999999999998E-2</v>
+      </c>
+      <c r="M18">
+        <f>0.00622+0.0725</f>
+        <v>7.8719999999999998E-2</v>
+      </c>
+      <c r="N18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>12</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <f>0.00622+0.06323</f>
+        <v>6.9449999999999998E-2</v>
+      </c>
+      <c r="M19">
+        <f>0.00622+0.06323</f>
+        <v>6.9449999999999998E-2</v>
+      </c>
+      <c r="N19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>12</v>
+      </c>
+      <c r="I20">
+        <v>20</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <f>0.02908+0.06074</f>
+        <v>8.9820000000000011E-2</v>
+      </c>
+      <c r="M20">
+        <f>0.02908+0.06074</f>
+        <v>8.9820000000000011E-2</v>
+      </c>
+      <c r="N20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>20</v>
+      </c>
+      <c r="I21">
+        <v>24</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21">
+        <f>0.00622+0.06323</f>
+        <v>6.9449999999999998E-2</v>
+      </c>
+      <c r="M21">
+        <f>0.00622+0.06323</f>
+        <v>6.9449999999999998E-2</v>
+      </c>
+      <c r="N21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>24</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+      <c r="L22">
+        <f>0.00622+0.06323</f>
+        <v>6.9449999999999998E-2</v>
+      </c>
+      <c r="M22">
+        <f>0.00622+0.06323</f>
+        <v>6.9449999999999998E-2</v>
+      </c>
+      <c r="N22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>12</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <f>0.00622+0.05557</f>
+        <v>6.1789999999999998E-2</v>
+      </c>
+      <c r="M23">
+        <f>0.00622+0.05557</f>
+        <v>6.1789999999999998E-2</v>
+      </c>
+      <c r="N23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>12</v>
+      </c>
+      <c r="I24">
+        <v>20</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <f>0.02908+0.06386</f>
+        <v>9.2939999999999995E-2</v>
+      </c>
+      <c r="M24">
+        <f>0.02908+0.06386</f>
+        <v>9.2939999999999995E-2</v>
+      </c>
+      <c r="N24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <v>20</v>
+      </c>
+      <c r="I25">
+        <v>24</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <f>0.00622+0.05557</f>
+        <v>6.1789999999999998E-2</v>
+      </c>
+      <c r="M25">
+        <f>0.00622+0.05557</f>
+        <v>6.1789999999999998E-2</v>
+      </c>
+      <c r="N25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>24</v>
+      </c>
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <v>6</v>
+      </c>
+      <c r="L26">
+        <f>0.00622+0.05557</f>
+        <v>6.1789999999999998E-2</v>
+      </c>
+      <c r="M26">
+        <f>0.00622+0.05557</f>
+        <v>6.1789999999999998E-2</v>
+      </c>
+      <c r="N26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+      <c r="G27">
+        <v>7</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>12</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <f>0.00622+0.05264</f>
+        <v>5.8859999999999996E-2</v>
+      </c>
+      <c r="M27">
+        <f>0.00622+0.05264</f>
+        <v>5.8859999999999996E-2</v>
+      </c>
+      <c r="N27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>7</v>
+      </c>
+      <c r="H28">
+        <v>12</v>
+      </c>
+      <c r="I28">
+        <v>20</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <f>0.02908+0.07521</f>
+        <v>0.10428999999999999</v>
+      </c>
+      <c r="M28">
+        <f>0.02908+0.07521</f>
+        <v>0.10428999999999999</v>
+      </c>
+      <c r="N28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>20</v>
+      </c>
+      <c r="I29">
+        <v>24</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29">
+        <f>0.00622+0.05264</f>
+        <v>5.8859999999999996E-2</v>
+      </c>
+      <c r="M29">
+        <f>0.00622+0.05264</f>
+        <v>5.8859999999999996E-2</v>
+      </c>
+      <c r="N29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>24</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
+      </c>
+      <c r="K30">
+        <v>6</v>
+      </c>
+      <c r="L30">
+        <f>0.00622+0.05264</f>
+        <v>5.8859999999999996E-2</v>
+      </c>
+      <c r="M30">
+        <f>0.00622+0.05264</f>
+        <v>5.8859999999999996E-2</v>
+      </c>
+      <c r="N30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>8</v>
+      </c>
+      <c r="G31">
+        <v>8</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>12</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>4</v>
+      </c>
+      <c r="L31">
+        <f>0.00622+0.05123</f>
+        <v>5.7450000000000001E-2</v>
+      </c>
+      <c r="M31">
+        <f>0.00622+0.05123</f>
+        <v>5.7450000000000001E-2</v>
+      </c>
+      <c r="N31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>8</v>
+      </c>
+      <c r="G32">
+        <v>8</v>
+      </c>
+      <c r="H32">
+        <v>12</v>
+      </c>
+      <c r="I32">
+        <v>20</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <f>0.02908+0.07138</f>
+        <v>0.10045999999999999</v>
+      </c>
+      <c r="M32">
+        <f>0.02908+0.07138</f>
+        <v>0.10045999999999999</v>
+      </c>
+      <c r="N32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <v>8</v>
+      </c>
+      <c r="H33">
+        <v>20</v>
+      </c>
+      <c r="I33">
+        <v>24</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <f>0.00622+0.05123</f>
+        <v>5.7450000000000001E-2</v>
+      </c>
+      <c r="M33">
+        <f>0.00622+0.05123</f>
+        <v>5.7450000000000001E-2</v>
+      </c>
+      <c r="N33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>8</v>
+      </c>
+      <c r="G34">
+        <v>8</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>24</v>
+      </c>
+      <c r="J34">
+        <v>5</v>
+      </c>
+      <c r="K34">
+        <v>6</v>
+      </c>
+      <c r="L34">
+        <f>0.00622+0.05123</f>
+        <v>5.7450000000000001E-2</v>
+      </c>
+      <c r="M34">
+        <f>0.00622+0.05123</f>
+        <v>5.7450000000000001E-2</v>
+      </c>
+      <c r="N34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>9</v>
+      </c>
+      <c r="G35">
+        <v>9</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>12</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>4</v>
+      </c>
+      <c r="L35">
+        <f>0.00622+0.05032</f>
+        <v>5.6539999999999993E-2</v>
+      </c>
+      <c r="M35">
+        <f>0.00622+0.05032</f>
+        <v>5.6539999999999993E-2</v>
+      </c>
+      <c r="N35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>9</v>
+      </c>
+      <c r="G36">
+        <v>9</v>
+      </c>
+      <c r="H36">
+        <v>12</v>
+      </c>
+      <c r="I36">
+        <v>20</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+      <c r="L36">
+        <f>0.02908+0.0632</f>
+        <v>9.2280000000000001E-2</v>
+      </c>
+      <c r="M36">
+        <f>0.02908+0.0632</f>
+        <v>9.2280000000000001E-2</v>
+      </c>
+      <c r="N36" t="s">
+        <v>14</v>
+      </c>
+      <c r="O36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>9</v>
+      </c>
+      <c r="G37">
+        <v>9</v>
+      </c>
+      <c r="H37">
+        <v>20</v>
+      </c>
+      <c r="I37">
+        <v>24</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>4</v>
+      </c>
+      <c r="L37">
+        <f>0.00622+0.05032</f>
+        <v>5.6539999999999993E-2</v>
+      </c>
+      <c r="M37">
+        <f>0.00622+0.05032</f>
+        <v>5.6539999999999993E-2</v>
+      </c>
+      <c r="N37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>9</v>
+      </c>
+      <c r="G38">
+        <v>9</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>24</v>
+      </c>
+      <c r="J38">
+        <v>5</v>
+      </c>
+      <c r="K38">
+        <v>6</v>
+      </c>
+      <c r="L38">
+        <f>0.00622+0.05032</f>
+        <v>5.6539999999999993E-2</v>
+      </c>
+      <c r="M38">
+        <f>0.00622+0.05032</f>
+        <v>5.6539999999999993E-2</v>
+      </c>
+      <c r="N38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <v>10</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>12</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>4</v>
+      </c>
+      <c r="L39">
+        <f>0.00622+0.06389</f>
+        <v>7.0110000000000006E-2</v>
+      </c>
+      <c r="M39">
+        <f>0.00622+0.06389</f>
+        <v>7.0110000000000006E-2</v>
+      </c>
+      <c r="N39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+      <c r="G40">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>12</v>
+      </c>
+      <c r="I40">
+        <v>20</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>4</v>
+      </c>
+      <c r="L40">
+        <f>0.02908+0.07184</f>
+        <v>0.10092000000000001</v>
+      </c>
+      <c r="M40">
+        <f>0.02908+0.07184</f>
+        <v>0.10092000000000001</v>
+      </c>
+      <c r="N40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>10</v>
+      </c>
+      <c r="G41">
+        <v>10</v>
+      </c>
+      <c r="H41">
+        <v>20</v>
+      </c>
+      <c r="I41">
+        <v>24</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>4</v>
+      </c>
+      <c r="L41">
+        <f>0.00622+0.06389</f>
+        <v>7.0110000000000006E-2</v>
+      </c>
+      <c r="M41">
+        <f>0.00622+0.06389</f>
+        <v>7.0110000000000006E-2</v>
+      </c>
+      <c r="N41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>10</v>
+      </c>
+      <c r="G42">
+        <v>10</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>24</v>
+      </c>
+      <c r="J42">
+        <v>5</v>
+      </c>
+      <c r="K42">
+        <v>6</v>
+      </c>
+      <c r="L42">
+        <f>0.00622+0.06389</f>
+        <v>7.0110000000000006E-2</v>
+      </c>
+      <c r="M42">
+        <f>0.00622+0.06389</f>
+        <v>7.0110000000000006E-2</v>
+      </c>
+      <c r="N42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>11</v>
+      </c>
+      <c r="G43">
+        <v>11</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>12</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>4</v>
+      </c>
+      <c r="L43">
+        <f>0.00622+0.0761</f>
+        <v>8.2320000000000004E-2</v>
+      </c>
+      <c r="M43">
+        <f>0.00622+0.0761</f>
+        <v>8.2320000000000004E-2</v>
+      </c>
+      <c r="N43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>11</v>
+      </c>
+      <c r="G44">
+        <v>11</v>
+      </c>
+      <c r="H44">
+        <v>12</v>
+      </c>
+      <c r="I44">
+        <v>20</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>4</v>
+      </c>
+      <c r="L44">
+        <f>0.02908+0.08491</f>
+        <v>0.11399000000000001</v>
+      </c>
+      <c r="M44">
+        <f>0.02908+0.08491</f>
+        <v>0.11399000000000001</v>
+      </c>
+      <c r="N44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>11</v>
+      </c>
+      <c r="G45">
+        <v>11</v>
+      </c>
+      <c r="H45">
+        <v>20</v>
+      </c>
+      <c r="I45">
+        <v>24</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>4</v>
+      </c>
+      <c r="L45">
+        <f>0.00622+0.0761</f>
+        <v>8.2320000000000004E-2</v>
+      </c>
+      <c r="M45">
+        <f>0.00622+0.0761</f>
+        <v>8.2320000000000004E-2</v>
+      </c>
+      <c r="N45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>11</v>
+      </c>
+      <c r="G46">
+        <v>11</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>24</v>
+      </c>
+      <c r="J46">
+        <v>5</v>
+      </c>
+      <c r="K46">
+        <v>6</v>
+      </c>
+      <c r="L46">
+        <f>0.00622+0.0761</f>
+        <v>8.2320000000000004E-2</v>
+      </c>
+      <c r="M46">
+        <f>0.00622+0.0761</f>
+        <v>8.2320000000000004E-2</v>
+      </c>
+      <c r="N46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>12</v>
+      </c>
+      <c r="G47">
+        <v>12</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>12</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>4</v>
+      </c>
+      <c r="L47">
+        <f>0.00622+0.10132</f>
+        <v>0.10754</v>
+      </c>
+      <c r="M47">
+        <f>0.00622+0.10132</f>
+        <v>0.10754</v>
+      </c>
+      <c r="N47" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>12</v>
+      </c>
+      <c r="G48">
+        <v>12</v>
+      </c>
+      <c r="H48">
+        <v>12</v>
+      </c>
+      <c r="I48">
+        <v>20</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>4</v>
+      </c>
+      <c r="L48">
+        <f>0.02908+0.11438</f>
+        <v>0.14346</v>
+      </c>
+      <c r="M48">
+        <f>0.02908+0.11438</f>
+        <v>0.14346</v>
+      </c>
+      <c r="N48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>12</v>
+      </c>
+      <c r="G49">
+        <v>12</v>
+      </c>
+      <c r="H49">
+        <v>20</v>
+      </c>
+      <c r="I49">
+        <v>24</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>4</v>
+      </c>
+      <c r="L49">
+        <f>0.00622+0.10132</f>
+        <v>0.10754</v>
+      </c>
+      <c r="M49">
+        <f>0.00622+0.10132</f>
+        <v>0.10754</v>
+      </c>
+      <c r="N49" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>12</v>
+      </c>
+      <c r="G50">
+        <v>12</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>24</v>
+      </c>
+      <c r="J50">
+        <v>5</v>
+      </c>
+      <c r="K50">
+        <v>6</v>
+      </c>
+      <c r="L50">
+        <f>0.00622+0.10132</f>
+        <v>0.10754</v>
+      </c>
+      <c r="M50">
+        <f>0.00622+0.10132</f>
+        <v>0.10754</v>
+      </c>
+      <c r="N50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>24</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>6</v>
-      </c>
-      <c r="L7">
+      <c r="G51">
+        <v>12</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>24</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>6</v>
+      </c>
+      <c r="L51">
         <f>10.5+0.55+7.53-0.51</f>
         <v>18.07</v>
       </c>
-      <c r="M7">
+      <c r="M51">
         <f>10.5+0.55+7.53-0.51</f>
         <v>18.07</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N51" t="s">
         <v>17</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O51" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Switched to August 2022 fixed rate contract for Oncor, CenterPoint
</commit_message>
<xml_diff>
--- a/data/WWTP_Billing.xlsx
+++ b/data/WWTP_Billing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Git/wwtp-energy-tariffs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0465C72D-D204-DD43-99A2-CDB3704F1787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74013B49-7315-DF46-A12A-6809EDA8629E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="61" activeTab="72" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="64" activeTab="75" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12000053001" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7589" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7589" uniqueCount="116">
   <si>
     <t>utility</t>
   </si>
@@ -461,12 +461,6 @@
     <t>Includes Schedule EECC for generation</t>
   </si>
   <si>
-    <t>Assumed a fixed rate contract at average annual LMP for Dallas zone</t>
-  </si>
-  <si>
-    <t>Assumed a fixed rate contract at average annual LMP for Houston zone</t>
-  </si>
-  <si>
     <t>Monthly average of day-ahead price</t>
   </si>
   <si>
@@ -483,6 +477,9 @@
   </si>
   <si>
     <t>Monthly average of historical market price</t>
+  </si>
+  <si>
+    <t>Assumed a fixed rate contract at August 2022 rate</t>
   </si>
 </sst>
 </file>
@@ -2378,7 +2375,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -2424,7 +2421,7 @@
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -2470,7 +2467,7 @@
         <v>14</v>
       </c>
       <c r="O5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -2515,7 +2512,7 @@
         <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -2560,7 +2557,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -2605,7 +2602,7 @@
         <v>14</v>
       </c>
       <c r="O8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
@@ -2650,7 +2647,7 @@
         <v>14</v>
       </c>
       <c r="O9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -2695,7 +2692,7 @@
         <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -2740,7 +2737,7 @@
         <v>14</v>
       </c>
       <c r="O11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -2785,7 +2782,7 @@
         <v>14</v>
       </c>
       <c r="O12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -2830,7 +2827,7 @@
         <v>14</v>
       </c>
       <c r="O13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -2876,7 +2873,7 @@
         <v>14</v>
       </c>
       <c r="O14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -4028,7 +4025,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15073,7 +15070,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15306,7 +15303,7 @@
         <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -15350,7 +15347,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -15394,7 +15391,7 @@
         <v>14</v>
       </c>
       <c r="O8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -15438,7 +15435,7 @@
         <v>14</v>
       </c>
       <c r="O9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -15482,7 +15479,7 @@
         <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -15526,7 +15523,7 @@
         <v>14</v>
       </c>
       <c r="O11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -15570,7 +15567,7 @@
         <v>14</v>
       </c>
       <c r="O12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -15614,7 +15611,7 @@
         <v>14</v>
       </c>
       <c r="O13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -15658,7 +15655,7 @@
         <v>14</v>
       </c>
       <c r="O14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -15702,7 +15699,7 @@
         <v>14</v>
       </c>
       <c r="O15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -15746,7 +15743,7 @@
         <v>14</v>
       </c>
       <c r="O16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
@@ -15790,7 +15787,7 @@
         <v>14</v>
       </c>
       <c r="O17" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -24385,7 +24382,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L3" sqref="L3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24504,16 +24501,16 @@
         <v>6</v>
       </c>
       <c r="L3">
-        <v>2.878E-2</v>
+        <v>0.06</v>
       </c>
       <c r="M3">
-        <v>2.878E-2</v>
+        <v>0.06</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -34427,7 +34424,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -34471,7 +34468,7 @@
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -34515,7 +34512,7 @@
         <v>14</v>
       </c>
       <c r="O5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -34559,7 +34556,7 @@
         <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -34603,7 +34600,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -34647,7 +34644,7 @@
         <v>14</v>
       </c>
       <c r="O8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -34691,7 +34688,7 @@
         <v>14</v>
       </c>
       <c r="O9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -34735,7 +34732,7 @@
         <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -34779,7 +34776,7 @@
         <v>14</v>
       </c>
       <c r="O11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -34823,7 +34820,7 @@
         <v>14</v>
       </c>
       <c r="O12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -34867,7 +34864,7 @@
         <v>14</v>
       </c>
       <c r="O13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -34911,7 +34908,7 @@
         <v>14</v>
       </c>
       <c r="O14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -34960,7 +34957,7 @@
         <v>17</v>
       </c>
       <c r="O15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -48002,7 +47999,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="L3" sqref="L3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -48121,16 +48118,16 @@
         <v>6</v>
       </c>
       <c r="L3">
-        <v>3.0530000000000002E-2</v>
+        <v>0.06</v>
       </c>
       <c r="M3">
-        <v>3.0530000000000002E-2</v>
+        <v>0.06</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -52109,7 +52106,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -53029,7 +53026,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -54627,7 +54624,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -54792,16 +54789,16 @@
         <v>6</v>
       </c>
       <c r="L4">
-        <v>2.878E-2</v>
+        <v>0.06</v>
       </c>
       <c r="M4">
-        <v>2.878E-2</v>
+        <v>0.06</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -58397,7 +58394,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -58516,16 +58513,16 @@
         <v>6</v>
       </c>
       <c r="L3">
-        <v>2.878E-2</v>
+        <v>0.06</v>
       </c>
       <c r="M3">
-        <v>2.878E-2</v>
+        <v>0.06</v>
       </c>
       <c r="N3" t="s">
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -61565,7 +61562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -61736,7 +61733,7 @@
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -62334,7 +62331,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -63343,8 +63340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -63509,16 +63506,16 @@
         <v>6</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="N4" t="s">
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -77752,7 +77749,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -77798,7 +77795,7 @@
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -77844,7 +77841,7 @@
         <v>14</v>
       </c>
       <c r="O5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -77889,7 +77886,7 @@
         <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -77934,7 +77931,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -77979,7 +77976,7 @@
         <v>14</v>
       </c>
       <c r="O8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
@@ -78024,7 +78021,7 @@
         <v>14</v>
       </c>
       <c r="O9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -78069,7 +78066,7 @@
         <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -78114,7 +78111,7 @@
         <v>14</v>
       </c>
       <c r="O11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -78159,7 +78156,7 @@
         <v>14</v>
       </c>
       <c r="O12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -78204,7 +78201,7 @@
         <v>14</v>
       </c>
       <c r="O13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -78250,7 +78247,7 @@
         <v>14</v>
       </c>
       <c r="O14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -79831,7 +79828,7 @@
         <v>14</v>
       </c>
       <c r="O3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -79877,7 +79874,7 @@
         <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -79923,7 +79920,7 @@
         <v>14</v>
       </c>
       <c r="O5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -79968,7 +79965,7 @@
         <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -80013,7 +80010,7 @@
         <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -80058,7 +80055,7 @@
         <v>14</v>
       </c>
       <c r="O8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
@@ -80103,7 +80100,7 @@
         <v>14</v>
       </c>
       <c r="O9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -80148,7 +80145,7 @@
         <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -80193,7 +80190,7 @@
         <v>14</v>
       </c>
       <c r="O11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -80238,7 +80235,7 @@
         <v>14</v>
       </c>
       <c r="O12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -80283,7 +80280,7 @@
         <v>14</v>
       </c>
       <c r="O13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -80329,7 +80326,7 @@
         <v>14</v>
       </c>
       <c r="O14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>